<commit_message>
Updated Time_Chart & Class Diagram
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -810,7 +810,7 @@
         <v>82.390243902439025</v>
       </c>
       <c r="J5">
-        <f>(G5/H5*100) - G5</f>
+        <f t="shared" ref="J5:J14" si="0">(G5/H5*100) - G5</f>
         <v>26.090243902439028</v>
       </c>
     </row>
@@ -839,11 +839,11 @@
         <v>75</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I13" si="0">(G6/H6*100)</f>
+        <f t="shared" ref="I6:I13" si="1">(G6/H6*100)</f>
         <v>57.066666666666663</v>
       </c>
       <c r="J6">
-        <f>(G6/H6*100) - G6</f>
+        <f t="shared" si="0"/>
         <v>14.266666666666666</v>
       </c>
     </row>
@@ -874,11 +874,11 @@
         <v>60</v>
       </c>
       <c r="I7">
+        <f t="shared" si="1"/>
+        <v>64.666666666666657</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
-        <v>64.666666666666657</v>
-      </c>
-      <c r="J7">
-        <f>(G7/H7*100) - G7</f>
         <v>25.86666666666666</v>
       </c>
     </row>
@@ -909,11 +909,11 @@
         <v>30</v>
       </c>
       <c r="I8">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="J8">
-        <f>(G8/H8*100) - G8</f>
         <v>9.3333333333333339</v>
       </c>
     </row>
@@ -944,11 +944,11 @@
         <v>80</v>
       </c>
       <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f>(G9/H9*100) - G9</f>
         <v>0</v>
       </c>
     </row>
@@ -981,11 +981,11 @@
         <v>50</v>
       </c>
       <c r="I10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="J10">
-        <f>(G10/H10*100) - G10</f>
         <v>13.5</v>
       </c>
     </row>
@@ -1006,11 +1006,11 @@
         <v>100</v>
       </c>
       <c r="I11">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="J11">
-        <f>(G11/H11*100) - G11</f>
         <v>0</v>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="J12">
-        <f>(G12/H12*100) - G12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1055,11 +1055,11 @@
         <v>0</v>
       </c>
       <c r="I13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" t="e">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" t="e">
-        <f>(G13/H13*100) - G13</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J14" t="e">
-        <f>(G14/H14*100) - G14</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P48" sqref="J1:P48"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1320,11 +1320,11 @@
       </c>
       <c r="T4" s="3">
         <f>(T12+T20+T28+T36+T44)</f>
+        <v>3.5</v>
+      </c>
+      <c r="U4" s="3">
+        <f>(U12+U20+U28+U36+U44)</f>
         <v>3</v>
-      </c>
-      <c r="U4" s="4">
-        <f>(U12+U20+U28+U36+U44)</f>
-        <v>0</v>
       </c>
       <c r="V4" s="4">
         <f>(V12+V20+V28+V36+V44)</f>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="Y4">
         <f>SUM(T4:X4)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1403,11 +1403,11 @@
       </c>
       <c r="T5" s="3">
         <f t="shared" ref="T5:X7" si="4">(T13+T21+T29+T37+T45)</f>
+        <v>3.5</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="4"/>
         <v>3</v>
-      </c>
-      <c r="U5" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
       <c r="V5" s="4">
         <f t="shared" si="4"/>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="Y5">
         <f>SUM(T5:X5)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1486,11 +1486,11 @@
       </c>
       <c r="T6" s="3">
         <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="4"/>
         <v>3</v>
-      </c>
-      <c r="U6" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
       <c r="V6" s="4">
         <f t="shared" si="4"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="Y6">
         <f>SUM(T6:X6)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="T7" s="3">
         <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="4"/>
         <v>3</v>
-      </c>
-      <c r="U7" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
       <c r="V7" s="4">
         <f t="shared" si="4"/>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="Y7">
         <f>SUM(T7:X7)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1636,7 +1636,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="12">
         <f>SUM(Y4:Y7)</f>
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1755,7 +1755,7 @@
         <v>19</v>
       </c>
       <c r="T12" s="3">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
@@ -1763,7 +1763,7 @@
       <c r="X12" s="4"/>
       <c r="Y12">
         <f>SUM(T12:X12)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1815,7 +1815,7 @@
         <v>22</v>
       </c>
       <c r="T13" s="7">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
@@ -1823,7 +1823,7 @@
       <c r="X13" s="4"/>
       <c r="Y13">
         <f>SUM(T13:X13)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1875,15 +1875,17 @@
         <v>23</v>
       </c>
       <c r="T14" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="U14" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="U14" s="3">
+        <v>1.5</v>
+      </c>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14">
         <f>SUM(T14:X14)</f>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -1935,15 +1937,17 @@
         <v>20</v>
       </c>
       <c r="T15" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="U15" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="U15" s="3">
+        <v>1.5</v>
+      </c>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15">
         <f>SUM(T15:X15)</f>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -1984,7 +1988,7 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="12">
         <f>SUM(Y12:Y15)</f>
-        <v>10.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2834,13 +2838,15 @@
         <v>19</v>
       </c>
       <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
+      <c r="U36" s="7">
+        <v>3</v>
+      </c>
       <c r="V36" s="5"/>
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
       <c r="Y36">
         <f>SUM(T36:X36)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -2891,16 +2897,18 @@
       <c r="S37" t="s">
         <v>22</v>
       </c>
-      <c r="T37" s="5">
+      <c r="T37" s="7">
         <v>0.5</v>
       </c>
-      <c r="U37" s="5"/>
+      <c r="U37" s="7">
+        <v>3</v>
+      </c>
       <c r="V37" s="5"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
       <c r="Y37">
         <f>SUM(T37:X37)</f>
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -3051,7 +3059,7 @@
       <c r="X40" s="6"/>
       <c r="Y40" s="12">
         <f>SUM(Y36:Y39)</f>
-        <v>0.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="41" spans="1:25">
@@ -3300,16 +3308,18 @@
       <c r="S46" t="s">
         <v>23</v>
       </c>
-      <c r="T46" s="6">
+      <c r="T46" s="3">
         <v>0.5</v>
       </c>
-      <c r="U46" s="6"/>
+      <c r="U46" s="3">
+        <v>1.5</v>
+      </c>
       <c r="V46" s="6"/>
       <c r="W46" s="4"/>
       <c r="X46" s="6"/>
       <c r="Y46">
         <f>SUM(T46:X46)</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:25">
@@ -3360,16 +3370,18 @@
       <c r="S47" t="s">
         <v>20</v>
       </c>
-      <c r="T47" s="6">
+      <c r="T47" s="3">
         <v>0.5</v>
       </c>
-      <c r="U47" s="6"/>
+      <c r="U47" s="3">
+        <v>1.5</v>
+      </c>
       <c r="V47" s="6"/>
       <c r="W47" s="6"/>
       <c r="X47" s="6"/>
       <c r="Y47">
         <f>SUM(T47:X47)</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:25">
@@ -3401,7 +3413,7 @@
       </c>
       <c r="Y48" s="12">
         <f>SUM(Y44:Y47)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:25">

</xml_diff>

<commit_message>
updated R4 and time chart
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="A4:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -897,11 +897,11 @@
       </c>
       <c r="F5">
         <f>(F6+F9+F10+F16+F17)</f>
-        <v>109.3</v>
+        <v>113.8</v>
       </c>
       <c r="G5" s="13">
         <f>((G6+G9+G10)/3)</f>
-        <v>89.566666666666663</v>
+        <v>91.066666666666663</v>
       </c>
       <c r="H5">
         <f>(H6+H9+H10)</f>
@@ -909,7 +909,7 @@
       </c>
       <c r="I5" s="14">
         <f>(I6+I9+I10)</f>
-        <v>11.574999999999994</v>
+        <v>7.6444444444444457</v>
       </c>
       <c r="J5" s="14"/>
     </row>
@@ -928,11 +928,11 @@
       </c>
       <c r="F6">
         <f>(F7+F8)</f>
-        <v>55.3</v>
+        <v>59.3</v>
       </c>
       <c r="G6" s="13">
         <f>(G7+G8)/2</f>
-        <v>92.5</v>
+        <v>95</v>
       </c>
       <c r="H6">
         <f>(H7+H8)</f>
@@ -940,7 +940,7 @@
       </c>
       <c r="I6" s="14">
         <f>(I7+I8)</f>
-        <v>8.6999999999999957</v>
+        <v>5.9222222222222243</v>
       </c>
       <c r="J6" s="14"/>
     </row>
@@ -961,17 +961,17 @@
         <v>41026</v>
       </c>
       <c r="F7">
-        <v>49.3</v>
+        <v>53.3</v>
       </c>
       <c r="G7" s="14">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H7">
         <v>150</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" ref="I7:I9" si="0">(F7/G7*100) - F7</f>
-        <v>8.6999999999999957</v>
+        <v>5.9222222222222243</v>
       </c>
       <c r="J7" s="14"/>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="G10" s="13">
         <f>((G11+G12+G13+G14+G15)/5)</f>
-        <v>76.2</v>
+        <v>78.2</v>
       </c>
       <c r="H10">
         <f>(SUM(H11:H15))</f>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="I10" s="14">
         <f>(SUM(I11:I15))</f>
-        <v>2.8749999999999982</v>
+        <v>1.7222222222222214</v>
       </c>
       <c r="J10" s="14"/>
     </row>
@@ -1197,17 +1197,17 @@
         <v>41026</v>
       </c>
       <c r="F15">
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
       <c r="G15" s="14">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H15">
         <v>4</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="1"/>
-        <v>2.8749999999999982</v>
+        <v>1.7222222222222214</v>
       </c>
       <c r="J15" s="14"/>
     </row>
@@ -1225,7 +1225,7 @@
         <v>41026</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="G16" s="14"/>
       <c r="I16" s="14"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F21">
         <f>SUM(F22:F31)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I21">
         <f>(SUM(I22:I31))</f>
@@ -1332,7 +1332,7 @@
         <v>41027</v>
       </c>
       <c r="F22">
-        <v>4.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:Y64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1738,11 +1738,11 @@
       </c>
       <c r="X4" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y4">
         <f>SUM(T4:X4)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1821,11 +1821,11 @@
       </c>
       <c r="X5" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y5">
         <f>SUM(T5:X5)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1904,11 +1904,11 @@
       </c>
       <c r="X6" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y6">
         <f>SUM(T6:X6)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1987,11 +1987,11 @@
       </c>
       <c r="X7" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="Y7">
         <f>SUM(T7:X7)</f>
-        <v>12.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -2038,7 +2038,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="12">
         <f>SUM(Y4:Y7)</f>
-        <v>57.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -2165,11 +2165,15 @@
       <c r="V12" s="3">
         <v>1</v>
       </c>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
+      <c r="W12" s="4">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>1</v>
+      </c>
       <c r="Y12">
         <f>SUM(T12:X12)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2229,11 +2233,15 @@
       <c r="V13" s="3">
         <v>1.5</v>
       </c>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
+      <c r="W13" s="4">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>1</v>
+      </c>
       <c r="Y13">
         <f>SUM(T13:X13)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2293,11 +2301,15 @@
       <c r="V14" s="3">
         <v>1.5</v>
       </c>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
+      <c r="W14" s="4">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>1</v>
+      </c>
       <c r="Y14">
         <f>SUM(T14:X14)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2357,11 +2369,15 @@
       <c r="V15" s="3">
         <v>1</v>
       </c>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>1</v>
+      </c>
       <c r="Y15">
         <f>SUM(T15:X15)</f>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2402,7 +2418,7 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="12">
         <f>SUM(Y12:Y15)</f>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2541,7 +2557,9 @@
       <c r="W20" s="3">
         <v>1</v>
       </c>
-      <c r="X20" s="6"/>
+      <c r="X20" s="6">
+        <v>0</v>
+      </c>
       <c r="Y20">
         <f>SUM(T20:X20)</f>
         <v>1</v>
@@ -2605,7 +2623,9 @@
       <c r="W21" s="3">
         <v>1</v>
       </c>
-      <c r="X21" s="6"/>
+      <c r="X21" s="6">
+        <v>0</v>
+      </c>
       <c r="Y21">
         <f>SUM(T21:X21)</f>
         <v>1</v>
@@ -2669,7 +2689,9 @@
       <c r="W22" s="3">
         <v>1</v>
       </c>
-      <c r="X22" s="6"/>
+      <c r="X22" s="6">
+        <v>0</v>
+      </c>
       <c r="Y22">
         <f>SUM(T22:X22)</f>
         <v>1</v>
@@ -2730,8 +2752,12 @@
         <v>0</v>
       </c>
       <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
+      <c r="W23" s="6">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6">
+        <v>0</v>
+      </c>
       <c r="Y23">
         <f>SUM(T23:X23)</f>
         <v>0</v>
@@ -2915,7 +2941,9 @@
       <c r="W28" s="3">
         <v>0.5</v>
       </c>
-      <c r="X28" s="6"/>
+      <c r="X28" s="6">
+        <v>0</v>
+      </c>
       <c r="Y28">
         <f>SUM(T28:X28)</f>
         <v>0.5</v>
@@ -2979,7 +3007,9 @@
       <c r="W29" s="3">
         <v>1.5</v>
       </c>
-      <c r="X29" s="6"/>
+      <c r="X29" s="6">
+        <v>0</v>
+      </c>
       <c r="Y29">
         <f>SUM(T29:X29)</f>
         <v>1.5</v>
@@ -3043,7 +3073,9 @@
       <c r="W30" s="3">
         <v>1.5</v>
       </c>
-      <c r="X30" s="6"/>
+      <c r="X30" s="6">
+        <v>0</v>
+      </c>
       <c r="Y30">
         <f>SUM(T30:X30)</f>
         <v>1.5</v>
@@ -3104,8 +3136,12 @@
         <v>0</v>
       </c>
       <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
+      <c r="W31" s="6">
+        <v>0</v>
+      </c>
+      <c r="X31" s="6">
+        <v>0</v>
+      </c>
       <c r="Y31">
         <f>SUM(T31:X31)</f>
         <v>0</v>
@@ -3284,11 +3320,15 @@
         <v>3</v>
       </c>
       <c r="V36" s="5"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
+      <c r="W36" s="4">
+        <v>0</v>
+      </c>
+      <c r="X36" s="3">
+        <v>1</v>
+      </c>
       <c r="Y36">
         <f>SUM(T36:X36)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -3348,11 +3388,15 @@
       <c r="V37" s="7">
         <v>0.5</v>
       </c>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
+      <c r="W37" s="4">
+        <v>0</v>
+      </c>
+      <c r="X37" s="3">
+        <v>1</v>
+      </c>
       <c r="Y37">
         <f>SUM(T37:X37)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -3408,11 +3452,15 @@
       <c r="V38" s="7">
         <v>0.5</v>
       </c>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
+      <c r="W38" s="4">
+        <v>0</v>
+      </c>
+      <c r="X38" s="3">
+        <v>1</v>
+      </c>
       <c r="Y38">
         <f>SUM(T38:X38)</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:25">
@@ -3468,11 +3516,15 @@
         <v>0</v>
       </c>
       <c r="V39" s="5"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
+      <c r="W39" s="4">
+        <v>0</v>
+      </c>
+      <c r="X39" s="3">
+        <v>1</v>
+      </c>
       <c r="Y39">
         <f>SUM(T39:X39)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:25">
@@ -3509,7 +3561,7 @@
       <c r="X40" s="6"/>
       <c r="Y40" s="12">
         <f>SUM(Y36:Y39)</f>
-        <v>7.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="41" spans="1:25">
@@ -3644,9 +3696,15 @@
       <c r="U44" s="6">
         <v>0</v>
       </c>
-      <c r="V44" s="6"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="6"/>
+      <c r="V44" s="6">
+        <v>0</v>
+      </c>
+      <c r="W44" s="4">
+        <v>0</v>
+      </c>
+      <c r="X44" s="6">
+        <v>0</v>
+      </c>
       <c r="Y44">
         <f>SUM(T44:X44)</f>
         <v>0</v>
@@ -3706,9 +3764,15 @@
       <c r="U45" s="6">
         <v>0</v>
       </c>
-      <c r="V45" s="6"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="6"/>
+      <c r="V45" s="6">
+        <v>0</v>
+      </c>
+      <c r="W45" s="4">
+        <v>0</v>
+      </c>
+      <c r="X45" s="6">
+        <v>0</v>
+      </c>
       <c r="Y45">
         <f>SUM(T45:X45)</f>
         <v>0</v>
@@ -3768,9 +3832,15 @@
       <c r="U46" s="3">
         <v>1.5</v>
       </c>
-      <c r="V46" s="6"/>
-      <c r="W46" s="4"/>
-      <c r="X46" s="6"/>
+      <c r="V46" s="6">
+        <v>0</v>
+      </c>
+      <c r="W46" s="4">
+        <v>0</v>
+      </c>
+      <c r="X46" s="6">
+        <v>0</v>
+      </c>
       <c r="Y46">
         <f>SUM(T46:X46)</f>
         <v>2</v>
@@ -3830,9 +3900,15 @@
       <c r="U47" s="3">
         <v>1.5</v>
       </c>
-      <c r="V47" s="6"/>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6"/>
+      <c r="V47" s="6">
+        <v>0</v>
+      </c>
+      <c r="W47" s="6">
+        <v>0</v>
+      </c>
+      <c r="X47" s="6">
+        <v>0</v>
+      </c>
       <c r="Y47">
         <f>SUM(T47:X47)</f>
         <v>2</v>
@@ -3963,8 +4039,12 @@
       <c r="V52" s="3">
         <v>1</v>
       </c>
-      <c r="W52" s="4"/>
-      <c r="X52" s="6"/>
+      <c r="W52" s="4">
+        <v>0</v>
+      </c>
+      <c r="X52" s="6">
+        <v>0</v>
+      </c>
       <c r="Y52">
         <f>SUM(T52:X52)</f>
         <v>2</v>
@@ -3978,9 +4058,15 @@
       <c r="U53" s="3">
         <v>1</v>
       </c>
-      <c r="V53" s="6"/>
-      <c r="W53" s="4"/>
-      <c r="X53" s="6"/>
+      <c r="V53" s="6">
+        <v>0</v>
+      </c>
+      <c r="W53" s="4">
+        <v>0</v>
+      </c>
+      <c r="X53" s="6">
+        <v>0</v>
+      </c>
       <c r="Y53">
         <f>SUM(T53:X53)</f>
         <v>1</v>
@@ -3994,9 +4080,15 @@
       <c r="U54" s="6">
         <v>0</v>
       </c>
-      <c r="V54" s="6"/>
-      <c r="W54" s="4"/>
-      <c r="X54" s="6"/>
+      <c r="V54" s="6">
+        <v>0</v>
+      </c>
+      <c r="W54" s="4">
+        <v>0</v>
+      </c>
+      <c r="X54" s="6">
+        <v>0</v>
+      </c>
       <c r="Y54">
         <f>SUM(T54:X54)</f>
         <v>0</v>
@@ -4010,18 +4102,24 @@
       <c r="U55" s="6">
         <v>0</v>
       </c>
-      <c r="V55" s="6"/>
-      <c r="W55" s="6"/>
-      <c r="X55" s="6"/>
+      <c r="V55" s="6">
+        <v>0</v>
+      </c>
+      <c r="W55" s="6">
+        <v>0</v>
+      </c>
+      <c r="X55" s="3">
+        <v>0.5</v>
+      </c>
       <c r="Y55">
         <f>SUM(T55:X55)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:25">
       <c r="Y56" s="12">
         <f>SUM(Y52:Y55)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="58" spans="1:25">
@@ -4059,11 +4157,15 @@
       <c r="V60" s="3">
         <v>3</v>
       </c>
-      <c r="W60" s="4"/>
-      <c r="X60" s="6"/>
+      <c r="W60" s="4">
+        <v>0</v>
+      </c>
+      <c r="X60" s="3">
+        <v>2</v>
+      </c>
       <c r="Y60">
         <f>SUM(T60:X60)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:25">
@@ -4079,11 +4181,15 @@
       <c r="V61" s="3">
         <v>3</v>
       </c>
-      <c r="W61" s="4"/>
-      <c r="X61" s="6"/>
+      <c r="W61" s="4">
+        <v>0</v>
+      </c>
+      <c r="X61" s="3">
+        <v>2</v>
+      </c>
       <c r="Y61">
         <f>SUM(T61:X61)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:25">
@@ -4099,11 +4205,15 @@
       <c r="V62" s="3">
         <v>3</v>
       </c>
-      <c r="W62" s="4"/>
-      <c r="X62" s="6"/>
+      <c r="W62" s="4">
+        <v>0</v>
+      </c>
+      <c r="X62" s="3">
+        <v>2</v>
+      </c>
       <c r="Y62">
         <f>SUM(T62:X62)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:25">
@@ -4119,17 +4229,21 @@
       <c r="V63" s="3">
         <v>4</v>
       </c>
-      <c r="W63" s="6"/>
-      <c r="X63" s="6"/>
+      <c r="W63" s="6">
+        <v>0</v>
+      </c>
+      <c r="X63" s="3">
+        <v>2</v>
+      </c>
       <c r="Y63">
         <f>SUM(T63:X63)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:25">
       <c r="Y64" s="12">
         <f>SUM(Y60:Y63)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed R5 in time chart as well as added R5.docx
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="98">
   <si>
     <t>Task1</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>L2-05</t>
+  </si>
+  <si>
+    <t>Week 17</t>
+  </si>
+  <si>
+    <t>R5</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:Y64"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1584,7 +1590,7 @@
     <col min="25" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1603,8 +1609,14 @@
       <c r="T1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
       <c r="C2" t="s">
         <v>39</v>
       </c>
@@ -1614,8 +1626,11 @@
       <c r="U2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="AD2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
       <c r="B3" t="s">
         <v>40</v>
       </c>
@@ -1661,8 +1676,23 @@
       <c r="X3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="AC3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1744,29 +1774,56 @@
         <f>SUM(T4:X4)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="AB4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC4" s="3">
+        <f>(AC12+AC20+AC28+AC36+AC44+AC52+AC60)</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <f t="shared" ref="AD4:AG4" si="2">(AD12+AD20+AD28+AD36+AD44+AD52+AD60)</f>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f>SUM(AC4:AG4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:E8" si="2">(B13+B21+B29+B37+B45+B53)</f>
+        <f t="shared" ref="B5:E8" si="3">(B13+B21+B29+B37+B45+B53)</f>
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F7" si="3">(F13+F21+F29+F37+F45)</f>
+        <f t="shared" ref="F5:F7" si="4">(F13+F21+F29+F37+F45)</f>
         <v>0</v>
       </c>
       <c r="G5" s="4">
@@ -1777,23 +1834,23 @@
         <v>21</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:O7" si="4">(K13+K21+K29+K37+K45)</f>
+        <f t="shared" ref="K5:O7" si="5">(K13+K21+K29+K37+K45)</f>
         <v>0</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P5">
@@ -1804,52 +1861,79 @@
         <v>21</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" ref="T5:X5" si="5">(T13+T21+T29+T37+T45+T53+T61)</f>
+        <f t="shared" ref="T5:X5" si="6">(T13+T21+T29+T37+T45+T53+T61)</f>
         <v>3.5</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="Y5">
         <f>SUM(T5:X5)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="AB5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" ref="AC5:AG5" si="7">(AC13+AC21+AC29+AC37+AC45+AC53+AC61)</f>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f>SUM(AC5:AG5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="4">
@@ -1860,23 +1944,23 @@
         <v>22</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.1</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P6">
@@ -1887,52 +1971,79 @@
         <v>22</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" ref="T6:X6" si="6">(T14+T22+T30+T38+T46+T54+T62)</f>
+        <f t="shared" ref="T6:X6" si="8">(T14+T22+T30+T38+T46+T54+T62)</f>
         <v>3.5</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="V6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="W6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="Y6">
         <f>SUM(T6:X6)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="AB6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" ref="AC6:AG6" si="9">(AC14+AC22+AC30+AC38+AC46+AC54+AC62)</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <f>SUM(AC6:AG6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G7" s="4">
@@ -1943,23 +2054,23 @@
         <v>19</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7">
@@ -1970,48 +2081,75 @@
         <v>19</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" ref="T7:X7" si="7">(T15+T23+T31+T39+T47+T55+T63)</f>
+        <f t="shared" ref="T7:X7" si="10">(T15+T23+T31+T39+T47+T55+T63)</f>
         <v>3.5</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="V7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="W7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
       <c r="Y7">
         <f>SUM(T7:X7)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="AB7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" ref="AC7:AG7" si="11">(AC15+AC23+AC31+AC39+AC47+AC55+AC63)</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <f>SUM(AC7:AG7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -2040,14 +2178,23 @@
         <f>SUM(Y4:Y7)</f>
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="12">
+        <f>SUM(AH4:AH7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
       <c r="G9" s="11">
         <f>SUM(G4:G8)</f>
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:34">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -2058,8 +2205,11 @@
       <c r="U10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="AD10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>40</v>
@@ -2107,8 +2257,23 @@
       <c r="X11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="AC11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -2175,8 +2340,11 @@
         <f>SUM(T12:X12)</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="AB12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -2243,8 +2411,11 @@
         <f>SUM(T13:X13)</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="AB13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -2311,8 +2482,11 @@
         <f>SUM(T14:X14)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="AB14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -2379,8 +2553,11 @@
         <f>SUM(T15:X15)</f>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="AB15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34">
       <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
@@ -2420,8 +2597,16 @@
         <f>SUM(Y12:Y15)</f>
         <v>26.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="12">
+        <f>SUM(AH12:AH15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2433,7 +2618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:34">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -2449,8 +2634,11 @@
       <c r="U18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="AD18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>40</v>
@@ -2498,8 +2686,23 @@
       <c r="X19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="AC19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -2564,8 +2767,11 @@
         <f>SUM(T20:X20)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="AB20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
@@ -2630,8 +2836,11 @@
         <f>SUM(T21:X21)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="AB21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
@@ -2696,8 +2905,11 @@
         <f>SUM(T22:X22)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="AB22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
@@ -2762,8 +2974,11 @@
         <f>SUM(T23:X23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="AB23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
@@ -2804,8 +3019,17 @@
         <f>SUM(Y20:Y23)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="12">
+        <f>SUM(AH20:AH23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2817,7 +3041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:34">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -2833,8 +3057,11 @@
       <c r="U26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:25">
+      <c r="AD26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>40</v>
@@ -2882,8 +3109,23 @@
       <c r="X27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:25">
+      <c r="AC27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2948,8 +3190,11 @@
         <f>SUM(T28:X28)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:25">
+      <c r="AB28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29" s="5" t="s">
         <v>21</v>
       </c>
@@ -3014,8 +3259,11 @@
         <f>SUM(T29:X29)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:25">
+      <c r="AB29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30" s="5" t="s">
         <v>22</v>
       </c>
@@ -3080,8 +3328,11 @@
         <f>SUM(T30:X30)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:25">
+      <c r="AB30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34">
       <c r="A31" s="5" t="s">
         <v>19</v>
       </c>
@@ -3146,8 +3397,11 @@
         <f>SUM(T31:X31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="AB31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34">
       <c r="A32" s="5" t="s">
         <v>45</v>
       </c>
@@ -3188,8 +3442,17 @@
         <f>SUM(Y28:Y31)</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:25">
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
+      <c r="AG32" s="6"/>
+      <c r="AH32" s="12">
+        <f>SUM(AH28:AH31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3201,7 +3464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:34">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -3217,8 +3480,11 @@
       <c r="U34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:25">
+      <c r="AD34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>40</v>
@@ -3266,8 +3532,23 @@
       <c r="X35" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:25">
+      <c r="AC35" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34">
       <c r="A36" s="5" t="s">
         <v>18</v>
       </c>
@@ -3330,8 +3611,11 @@
         <f>SUM(T36:X36)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:25">
+      <c r="AB36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34">
       <c r="A37" s="5" t="s">
         <v>21</v>
       </c>
@@ -3398,8 +3682,11 @@
         <f>SUM(T37:X37)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:25">
+      <c r="AB37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34">
       <c r="A38" s="5" t="s">
         <v>22</v>
       </c>
@@ -3462,8 +3749,11 @@
         <f>SUM(T38:X38)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:25">
+      <c r="AB38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34">
       <c r="A39" s="5" t="s">
         <v>19</v>
       </c>
@@ -3526,8 +3816,11 @@
         <f>SUM(T39:X39)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:25">
+      <c r="AB39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34">
       <c r="A40" s="5" t="s">
         <v>45</v>
       </c>
@@ -3563,8 +3856,15 @@
         <f>SUM(Y36:Y39)</f>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:25">
+      <c r="AC40" s="5"/>
+      <c r="AF40" s="6"/>
+      <c r="AG40" s="6"/>
+      <c r="AH40" s="12">
+        <f>SUM(AH36:AH39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3576,7 +3876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:34">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -3592,8 +3892,11 @@
       <c r="U42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:25">
+      <c r="AD42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>40</v>
@@ -3641,8 +3944,23 @@
       <c r="X43" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:25">
+      <c r="AC43" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34">
       <c r="A44" s="5" t="s">
         <v>18</v>
       </c>
@@ -3709,8 +4027,11 @@
         <f>SUM(T44:X44)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:25">
+      <c r="AB44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34">
       <c r="A45" s="5" t="s">
         <v>21</v>
       </c>
@@ -3777,8 +4098,11 @@
         <f>SUM(T45:X45)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:25">
+      <c r="AB45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34">
       <c r="A46" s="5" t="s">
         <v>22</v>
       </c>
@@ -3845,8 +4169,11 @@
         <f>SUM(T46:X46)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:25">
+      <c r="AB46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -3913,8 +4240,11 @@
         <f>SUM(T47:X47)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:25">
+      <c r="AB47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34">
       <c r="A48" s="5" t="s">
         <v>45</v>
       </c>
@@ -3945,14 +4275,18 @@
         <f>SUM(Y44:Y47)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:25">
+      <c r="AH48" s="12">
+        <f>SUM(AH44:AH47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34">
       <c r="G49" s="12">
         <f>SUM(G44:G48)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:34">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="8"/>
@@ -3974,8 +4308,11 @@
       <c r="U50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:25">
+      <c r="AD50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34">
       <c r="A51" s="5"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -4009,8 +4346,23 @@
       <c r="X51" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="52" spans="1:25">
+      <c r="AC51" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -4049,8 +4401,11 @@
         <f>SUM(T52:X52)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:25">
+      <c r="AB52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34">
       <c r="S53" t="s">
         <v>21</v>
       </c>
@@ -4071,8 +4426,11 @@
         <f>SUM(T53:X53)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:25">
+      <c r="AB53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34">
       <c r="S54" t="s">
         <v>22</v>
       </c>
@@ -4093,8 +4451,11 @@
         <f>SUM(T54:X54)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:25">
+      <c r="AB54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34">
       <c r="S55" t="s">
         <v>19</v>
       </c>
@@ -4115,19 +4476,29 @@
         <f>SUM(T55:X55)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:25">
+      <c r="AB55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34">
       <c r="Y56" s="12">
         <f>SUM(Y52:Y55)</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:25">
+      <c r="AH56" s="12">
+        <f>SUM(AH52:AH55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34">
       <c r="U58" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="59" spans="1:25">
+      <c r="AD58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34">
       <c r="T59" t="s">
         <v>40</v>
       </c>
@@ -4143,8 +4514,23 @@
       <c r="X59" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:25">
+      <c r="AC59" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34">
       <c r="S60" t="s">
         <v>18</v>
       </c>
@@ -4167,8 +4553,11 @@
         <f>SUM(T60:X60)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:25">
+      <c r="AB60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34">
       <c r="S61" t="s">
         <v>21</v>
       </c>
@@ -4191,8 +4580,11 @@
         <f>SUM(T61:X61)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:25">
+      <c r="AB61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34">
       <c r="S62" t="s">
         <v>22</v>
       </c>
@@ -4215,8 +4607,11 @@
         <f>SUM(T62:X62)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:25">
+      <c r="AB62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34">
       <c r="S63" t="s">
         <v>19</v>
       </c>
@@ -4239,11 +4634,18 @@
         <f>SUM(T63:X63)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:25">
+      <c r="AB63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34">
       <c r="Y64" s="12">
         <f>SUM(Y60:Y63)</f>
         <v>22</v>
+      </c>
+      <c r="AH64" s="12">
+        <f>SUM(AH60:AH63)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Time Chart again
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AC44" sqref="AC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="AC4" s="3">
         <f>(AC12+AC20+AC28+AC36+AC44+AC52+AC60)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD4" s="3">
         <f t="shared" ref="AD4:AG4" si="2">(AD12+AD20+AD28+AD36+AD44+AD52+AD60)</f>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="AH4">
         <f>SUM(AC4:AG4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="AD7" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="3">
         <f t="shared" si="11"/>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="AH7">
         <f>SUM(AC7:AG7)</f>
-        <v>2.2999999999999998</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -2363,7 +2363,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="12">
         <f>SUM(AH4:AH7)</f>
-        <v>9.3000000000000007</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -2733,6 +2733,13 @@
       </c>
       <c r="AB15" t="s">
         <v>15</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH15">
+        <f>SUM(AC15:AG15)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -2781,7 +2788,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="12">
         <f>SUM(AH12:AH15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -2948,6 +2955,13 @@
       <c r="AB20" t="s">
         <v>14</v>
       </c>
+      <c r="AC20">
+        <v>2</v>
+      </c>
+      <c r="AH20">
+        <f>SUM(AC20:AG20)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:34">
       <c r="A21" s="5" t="s">
@@ -3204,7 +3218,7 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="12">
         <f>SUM(AH20:AH23)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:34">
@@ -3371,6 +3385,13 @@
       <c r="AB28" t="s">
         <v>14</v>
       </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <f>SUM(AC28:AG28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:34">
       <c r="A29" s="5" t="s">
@@ -3577,6 +3598,10 @@
       </c>
       <c r="AB31" t="s">
         <v>15</v>
+      </c>
+      <c r="AH31">
+        <f>SUM(AC31:AG31)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:34">

</xml_diff>

<commit_message>
vi har fixat lite saker
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
+    <sheet name="Weekly Individual Progress" sheetId="3" r:id="rId2"/>
+    <sheet name="Percentage Done" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="103">
   <si>
     <t>L1</t>
   </si>
@@ -303,12 +304,36 @@
   </si>
   <si>
     <t xml:space="preserve">  Camera</t>
+  </si>
+  <si>
+    <t>Work Hours</t>
+  </si>
+  <si>
+    <t>Week 18</t>
+  </si>
+  <si>
+    <t>Week 19</t>
+  </si>
+  <si>
+    <t>Week 20</t>
+  </si>
+  <si>
+    <t>Week 21</t>
+  </si>
+  <si>
+    <t>Week 22</t>
+  </si>
+  <si>
+    <t>Percentage done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -357,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -386,6 +411,7 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -724,6 +750,9 @@
       <c r="H1" t="s">
         <v>79</v>
       </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -785,7 +814,7 @@
       </c>
       <c r="G5" s="13">
         <f>((G6+G9+G10)/3)</f>
-        <v>92.566666666666663</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <f>(H6+H9+H10)</f>
@@ -793,7 +822,7 @@
       </c>
       <c r="I5" s="14">
         <f>(I6+I9+I10)</f>
-        <v>3.189473684210526</v>
+        <v>0</v>
       </c>
       <c r="J5" s="14"/>
     </row>
@@ -817,7 +846,7 @@
       </c>
       <c r="G6" s="17">
         <f>(G7+G8)/2</f>
-        <v>97.5</v>
+        <v>100</v>
       </c>
       <c r="H6" s="7">
         <f>(H7+H8)</f>
@@ -825,7 +854,7 @@
       </c>
       <c r="I6" s="16">
         <f>(I7+I8)</f>
-        <v>3.189473684210526</v>
+        <v>0</v>
       </c>
       <c r="J6" s="14"/>
     </row>
@@ -849,14 +878,14 @@
         <v>60.6</v>
       </c>
       <c r="G7" s="14">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>150</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" ref="I7:I9" si="0">(F7/G7*100) - F7</f>
-        <v>3.189473684210526</v>
+        <v>0</v>
       </c>
       <c r="J7" s="14"/>
     </row>
@@ -943,8 +972,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="17">
-        <f>((G11+G12+G13+G14+G15)/5)</f>
-        <v>80.2</v>
+        <v>100</v>
       </c>
       <c r="H10" s="7">
         <f>(SUM(H11:H15))</f>
@@ -1057,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="14">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1185,8 +1213,8 @@
         <v>21</v>
       </c>
       <c r="G20" s="14">
-        <f>(G21+G32+G33+G36+G37+G38)/6</f>
-        <v>3.4166666666666665</v>
+        <f>(G21+G32+G33+G36)/4</f>
+        <v>5.125</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1196,9 +1224,6 @@
         <f>I21+I32+I33+I36+I37+I38</f>
         <v>71.291666666666671</v>
       </c>
-      <c r="J20">
-        <v>-160</v>
-      </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="7" t="s">
@@ -1230,9 +1255,6 @@
         <f>(SUM(I22:I31))</f>
         <v>71.291666666666671</v>
       </c>
-      <c r="J21">
-        <v>-184</v>
-      </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
@@ -1445,9 +1467,6 @@
       <c r="I28" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="J28">
-        <v>184</v>
       </c>
       <c r="N28" s="2"/>
     </row>
@@ -1732,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AC44" sqref="AC44"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4883,4 +4902,435 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <f>K4+K15+K16+K19+K20+K21</f>
+        <v>21</v>
+      </c>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="J4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="7">
+        <f>SUM(K5:K14)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="J6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="J7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="J13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="J14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="J15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="J16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="7">
+        <f>SUM(K17:K18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="J18" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="18">
+        <v>0</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="J19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="J20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="18">
+        <v>1</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="J21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished R5 and updated the time chart
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -356,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -388,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -419,6 +425,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H16:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I38" sqref="A4:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -817,7 +824,7 @@
       </c>
       <c r="F5">
         <f>(F6+F9+F10+F16+F17)</f>
-        <v>121.1</v>
+        <v>123.1</v>
       </c>
       <c r="G5" s="13">
         <f>((G6+G9+G10)/3)</f>
@@ -976,7 +983,7 @@
       </c>
       <c r="F10" s="7">
         <f>SUM(F11:F14)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G10" s="17">
         <v>100</v>
@@ -1089,7 +1096,7 @@
         <v>41029</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
         <v>100</v>
@@ -1217,11 +1224,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>5.125</v>
+        <v>6.875</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1229,7 +1236,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>71.291666666666671</v>
+        <v>67.791666666666671</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1248,11 +1255,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>17.5</v>
+        <v>24.5</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1260,7 +1267,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>71.291666666666671</v>
+        <v>67.791666666666671</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1280,17 +1287,17 @@
         <v>41027</v>
       </c>
       <c r="F22">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H22">
         <v>4.5</v>
       </c>
       <c r="I22" s="14">
         <f>(F22/G22*100) - F22</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1758,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20:AC23"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2215,15 +2222,15 @@
       </c>
       <c r="AF6" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG6" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f>SUM(AC6:AG6)</f>
-        <v>5.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -2389,7 +2396,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="12">
         <f>SUM(AH4:AH7)</f>
-        <v>20.3</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -2706,9 +2713,12 @@
       <c r="AD14" s="19">
         <v>3</v>
       </c>
+      <c r="AG14" s="20">
+        <v>1</v>
+      </c>
       <c r="AH14">
         <f>SUM(AD14:AG14)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -2835,7 +2845,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="12">
         <f>SUM(AH12:AH15)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -4897,6 +4907,12 @@
       <c r="AB62" t="s">
         <v>18</v>
       </c>
+      <c r="AF62" s="20">
+        <v>3</v>
+      </c>
+      <c r="AH62">
+        <v>3</v>
+      </c>
     </row>
     <row r="63" spans="1:34">
       <c r="S63" t="s">
@@ -4932,7 +4948,7 @@
       </c>
       <c r="AH64" s="12">
         <f>SUM(AH60:AH63)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4946,7 +4962,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="P21" sqref="A1:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
changes in gameObject,HUD,Candy,Ghost. Also added two .fx files
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="105">
   <si>
     <t>L1</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>Percentage done</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>Progammering</t>
   </si>
 </sst>
 </file>
@@ -356,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,12 +381,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -425,7 +425,6 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I38" sqref="A4:I38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1763,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH64"/>
+  <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AI21" sqref="AI21"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1799,9 +1798,12 @@
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:43">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1826,8 +1828,14 @@
       <c r="AC1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AK1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -1840,8 +1848,11 @@
       <c r="AD2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:34">
+      <c r="AM2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -1902,8 +1913,23 @@
       <c r="AG3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:34">
+      <c r="AL3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1993,27 +2019,54 @@
         <v>2</v>
       </c>
       <c r="AD4" s="3">
-        <f t="shared" ref="AD4:AG4" si="2">(AD12+AD20+AD28+AD36+AD44+AD52+AD60)</f>
+        <f>(AD12+AD20+AD28+AD36+AD44+AD52+AD60)</f>
         <v>3</v>
       </c>
       <c r="AE4" s="3">
-        <f t="shared" si="2"/>
+        <f>(AE12+AE20+AE28+AE36+AE44+AE52+AE60)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="3">
-        <f t="shared" si="2"/>
+        <f>(AF12+AF20+AF28+AF36+AF44+AF52+AF60)</f>
         <v>0</v>
       </c>
       <c r="AG4" s="3">
-        <f t="shared" si="2"/>
+        <f>(AG12+AG20+AG28+AG36+AG44+AG52+AG60)</f>
         <v>0</v>
       </c>
       <c r="AH4">
         <f>SUM(AC4:AG4)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:34">
+      <c r="AK4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL4">
+        <f>SUM(AL12,AL20,AL28,AL36)</f>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" ref="AM4:AQ4" si="2">SUM(AM12,AM20,AM28,AM36)</f>
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2099,31 +2152,58 @@
         <v>17</v>
       </c>
       <c r="AC5" s="3">
-        <f t="shared" ref="AC5:AG5" si="7">(AC13+AC21+AC29+AC37+AC45+AC53+AC61)</f>
+        <f>(AC13+AC21+AC29+AC37+AC45+AC53+AC61)</f>
         <v>2.5</v>
       </c>
       <c r="AD5" s="3">
-        <f t="shared" si="7"/>
+        <f>(AD13+AD21+AD29+AD37+AD45+AD53+AD61)</f>
         <v>3</v>
       </c>
       <c r="AE5" s="3">
-        <f t="shared" si="7"/>
+        <f>(AE13+AE21+AE29+AE37+AE45+AE53+AE61)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="3">
-        <f t="shared" si="7"/>
+        <f>(AF13+AF21+AF29+AF37+AF45+AF53+AF61)</f>
         <v>0</v>
       </c>
       <c r="AG5" s="3">
-        <f t="shared" si="7"/>
+        <f>(AG13+AG21+AG29+AG37+AG45+AG53+AG61)</f>
         <v>0</v>
       </c>
       <c r="AH5">
         <f>SUM(AC5:AG5)</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:34">
+      <c r="AK5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL5">
+        <f>SUM(AL13,AL21,AL29,AL37)</f>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" ref="AM5:AQ5" si="7">SUM(AM13,AM21,AM29,AM37)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2209,31 +2289,58 @@
         <v>18</v>
       </c>
       <c r="AC6" s="3">
-        <f t="shared" ref="AC6:AG6" si="9">(AC14+AC22+AC30+AC38+AC46+AC54+AC62)</f>
+        <f>(AC14+AC22+AC30+AC38+AC46+AC54+AC62)</f>
         <v>2.5</v>
       </c>
       <c r="AD6" s="3">
-        <f t="shared" si="9"/>
+        <f>(AD14+AD22+AD30+AD38+AD46+AD54+AD62)</f>
         <v>3</v>
       </c>
       <c r="AE6" s="3">
-        <f t="shared" si="9"/>
+        <f>(AE14+AE22+AE30+AE38+AE46+AE54+AE62)</f>
         <v>0</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" si="9"/>
+        <f>(AF14+AF22+AF30+AF38+AF46+AF54+AF62)</f>
         <v>3</v>
       </c>
       <c r="AG6" s="3">
-        <f t="shared" si="9"/>
+        <f>(AG14+AG22+AG30+AG38+AG46+AG54+AG62)</f>
         <v>1</v>
       </c>
       <c r="AH6">
         <f>SUM(AC6:AG6)</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:34">
+      <c r="AK6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL6">
+        <f>SUM(AL22,AL30,AL38,AL14)</f>
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" ref="AM6:AQ6" si="9">SUM(AM22,AM30,AM38,AM14)</f>
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2319,31 +2426,58 @@
         <v>15</v>
       </c>
       <c r="AC7" s="3">
-        <f t="shared" ref="AC7:AG7" si="11">(AC15+AC23+AC31+AC39+AC47+AC55+AC63)</f>
+        <f>(AC15+AC23+AC31+AC39+AC47+AC55+AC63)</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="AD7" s="3">
-        <f t="shared" si="11"/>
+        <f>(AD15+AD23+AD31+AD39+AD47+AD55+AD63)</f>
         <v>2</v>
       </c>
       <c r="AE7" s="3">
-        <f t="shared" si="11"/>
+        <f>(AE15+AE23+AE31+AE39+AE47+AE55+AE63)</f>
         <v>0</v>
       </c>
       <c r="AF7" s="3">
-        <f t="shared" si="11"/>
+        <f>(AF15+AF23+AF31+AF39+AF47+AF55+AF63)</f>
         <v>0</v>
       </c>
       <c r="AG7" s="3">
-        <f t="shared" si="11"/>
+        <f>(AG15+AG23+AG31+AG39+AG47+AG55+AG63)</f>
         <v>0</v>
       </c>
       <c r="AH7">
         <f>SUM(AC7:AG7)</f>
         <v>4.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:34">
+      <c r="AK7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL7">
+        <f>SUM(AL15,AL23,AL31,AL39)</f>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" ref="AM7:AQ7" si="11">SUM(AM15,AM23,AM31,AM39)</f>
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -2398,14 +2532,18 @@
         <f>SUM(AH4:AH7)</f>
         <v>24.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:34">
+      <c r="AQ8" s="12">
+        <f>SUM(AQ4:AQ7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="G9" s="11">
         <f>SUM(G4:G8)</f>
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:43">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -2419,8 +2557,11 @@
       <c r="AD10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:34">
+      <c r="AM10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>36</v>
@@ -2483,8 +2624,23 @@
       <c r="AG11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:34">
+      <c r="AL11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2561,8 +2717,30 @@
         <f>SUM(AD12:AG12)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:34">
+      <c r="AK12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <f>SUM(AL12:AP12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2639,8 +2817,30 @@
         <f>SUM(AD13:AG13)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:34">
+      <c r="AK13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <f>SUM(AL13:AP13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2713,15 +2913,37 @@
       <c r="AD14" s="19">
         <v>3</v>
       </c>
-      <c r="AG14" s="20">
+      <c r="AG14" s="7">
         <v>1</v>
       </c>
       <c r="AH14">
         <f>SUM(AD14:AG14)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:34">
+      <c r="AK14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <f>SUM(AL14:AP14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2798,8 +3020,30 @@
         <f>SUM(AD15:AG15)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:34">
+      <c r="AK15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <f>SUM(AL15:AP15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -2847,8 +3091,12 @@
         <f>SUM(AH12:AH15)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:34">
+      <c r="AQ16" s="12">
+        <f>SUM(AQ12:AQ15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2860,7 +3108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:43">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -2879,8 +3127,11 @@
       <c r="AD18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:34">
+      <c r="AM18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -2943,8 +3194,23 @@
       <c r="AG19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:34">
+      <c r="AL19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
@@ -3016,8 +3282,30 @@
         <f>SUM(AC20:AG20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:34">
+      <c r="AK20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20">
+        <f>SUM(AL20:AP20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -3089,8 +3377,30 @@
         <f>SUM(AC21:AG21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:34">
+      <c r="AK21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <f>SUM(AL21:AP21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
@@ -3162,8 +3472,30 @@
         <f>SUM(AC22:AG22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:34">
+      <c r="AK22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22">
+        <f>SUM(AL22:AP22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43">
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
@@ -3235,8 +3567,30 @@
         <f>SUM(AC23:AG23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:34">
+      <c r="AK23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <f>SUM(AL23:AP23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43">
       <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
@@ -3286,8 +3640,12 @@
         <f>SUM(AH20:AH23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:34">
+      <c r="AQ24" s="12">
+        <f>SUM(AQ20:AQ23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3299,7 +3657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:43">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -3318,8 +3676,11 @@
       <c r="AD26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:34">
+      <c r="AM26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>36</v>
@@ -3382,8 +3743,23 @@
       <c r="AG27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:34">
+      <c r="AL27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -3458,8 +3834,30 @@
         <f>SUM(AC28:AG28)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:34">
+      <c r="AK28" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
+      </c>
+      <c r="AM28">
+        <v>0</v>
+      </c>
+      <c r="AN28">
+        <v>0</v>
+      </c>
+      <c r="AO28">
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <v>0</v>
+      </c>
+      <c r="AQ28">
+        <f>SUM(AL28:AP28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -3527,8 +3925,30 @@
       <c r="AB29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:34">
+      <c r="AK29" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
+      </c>
+      <c r="AM29">
+        <v>0</v>
+      </c>
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <v>0</v>
+      </c>
+      <c r="AQ29">
+        <f>SUM(AL29:AP29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -3596,8 +4016,30 @@
       <c r="AB30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:34">
+      <c r="AK30" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL30">
+        <v>0</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <v>0</v>
+      </c>
+      <c r="AO30">
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <f>SUM(AL30:AP30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
@@ -3669,8 +4111,30 @@
         <f>SUM(AC31:AG31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:34">
+      <c r="AK31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <f>SUM(AL31:AP31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43">
       <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
@@ -3720,8 +4184,12 @@
         <f>SUM(AH28:AH31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:34">
+      <c r="AQ32" s="12">
+        <f>SUM(AQ28:AQ31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3733,7 +4201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:34">
+    <row r="34" spans="1:43">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -3752,8 +4220,11 @@
       <c r="AD34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:34">
+      <c r="AM34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
@@ -3816,8 +4287,23 @@
       <c r="AG35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:34">
+      <c r="AL35" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43">
       <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
@@ -3890,8 +4376,30 @@
         <f>SUM(AC36:AG36)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:34">
+      <c r="AK36" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+      <c r="AM36">
+        <v>0</v>
+      </c>
+      <c r="AN36">
+        <v>0</v>
+      </c>
+      <c r="AO36">
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <v>0</v>
+      </c>
+      <c r="AQ36">
+        <f>SUM(AL36:AP36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43">
       <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
@@ -3968,8 +4476,30 @@
         <f>SUM(AC37:AG37)</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:34">
+      <c r="AK37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
+      </c>
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AN37">
+        <v>0</v>
+      </c>
+      <c r="AO37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <f>SUM(AL37:AP37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43">
       <c r="A38" s="5" t="s">
         <v>18</v>
       </c>
@@ -4042,8 +4572,30 @@
         <f>SUM(AC38:AG38)</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:34">
+      <c r="AK38" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL38">
+        <v>0</v>
+      </c>
+      <c r="AM38">
+        <v>0</v>
+      </c>
+      <c r="AN38">
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <v>0</v>
+      </c>
+      <c r="AP38">
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <f>SUM(AL38:AP38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -4116,8 +4668,30 @@
         <f>SUM(AC39:AG39)</f>
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:34">
+      <c r="AK39" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL39">
+        <v>0</v>
+      </c>
+      <c r="AM39">
+        <v>0</v>
+      </c>
+      <c r="AN39">
+        <v>0</v>
+      </c>
+      <c r="AO39">
+        <v>0</v>
+      </c>
+      <c r="AP39">
+        <v>0</v>
+      </c>
+      <c r="AQ39">
+        <f>SUM(AL39:AP39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -4160,8 +4734,12 @@
         <f>SUM(AH36:AH39)</f>
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="41" spans="1:34">
+      <c r="AQ40" s="12">
+        <f>SUM(AQ36:AQ39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -4173,7 +4751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:34">
+    <row r="42" spans="1:43">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -4193,7 +4771,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:34">
+    <row r="43" spans="1:43">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>36</v>
@@ -4257,7 +4835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:34">
+    <row r="44" spans="1:43">
       <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
@@ -4328,7 +4906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:34">
+    <row r="45" spans="1:43">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -4399,7 +4977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:34">
+    <row r="46" spans="1:43">
       <c r="A46" s="5" t="s">
         <v>18</v>
       </c>
@@ -4470,7 +5048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:34">
+    <row r="47" spans="1:43">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -4541,7 +5119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:34">
+    <row r="48" spans="1:43">
       <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
@@ -4577,13 +5155,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:34">
+    <row r="49" spans="1:42">
       <c r="G49" s="12">
         <f>SUM(G44:G48)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="50" spans="1:34">
+    <row r="50" spans="1:42">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="8"/>
@@ -4609,7 +5187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:34">
+    <row r="51" spans="1:42">
       <c r="A51" s="5"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -4659,7 +5237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:34">
+    <row r="52" spans="1:42">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -4702,7 +5280,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:34">
+    <row r="53" spans="1:42">
       <c r="S53" t="s">
         <v>17</v>
       </c>
@@ -4727,7 +5305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:34">
+    <row r="54" spans="1:42">
       <c r="S54" t="s">
         <v>18</v>
       </c>
@@ -4752,7 +5330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:34">
+    <row r="55" spans="1:42">
       <c r="S55" t="s">
         <v>15</v>
       </c>
@@ -4777,7 +5355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:34">
+    <row r="56" spans="1:42">
       <c r="Y56" s="12">
         <f>SUM(Y52:Y55)</f>
         <v>3.5</v>
@@ -4787,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:34">
+    <row r="58" spans="1:42">
       <c r="U58" t="s">
         <v>47</v>
       </c>
@@ -4795,7 +5373,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:34">
+    <row r="59" spans="1:42">
       <c r="T59" t="s">
         <v>36</v>
       </c>
@@ -4827,7 +5405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:34">
+    <row r="60" spans="1:42">
       <c r="S60" t="s">
         <v>14</v>
       </c>
@@ -4854,7 +5432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:34">
+    <row r="61" spans="1:42">
       <c r="S61" t="s">
         <v>17</v>
       </c>
@@ -4881,7 +5459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:34">
+    <row r="62" spans="1:42">
       <c r="S62" t="s">
         <v>18</v>
       </c>
@@ -4907,14 +5485,15 @@
       <c r="AB62" t="s">
         <v>18</v>
       </c>
-      <c r="AF62" s="20">
+      <c r="AF62" s="7">
         <v>3</v>
       </c>
       <c r="AH62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:34">
+      <c r="AN62" s="5"/>
+    </row>
+    <row r="63" spans="1:42">
       <c r="S63" t="s">
         <v>15</v>
       </c>
@@ -4941,7 +5520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:34">
+    <row r="64" spans="1:42">
       <c r="Y64" s="12">
         <f>SUM(Y60:Y63)</f>
         <v>22</v>
@@ -4950,6 +5529,7 @@
         <f>SUM(AH60:AH63)</f>
         <v>3</v>
       </c>
+      <c r="AP64" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated time chart and R6
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>6.875</v>
+        <v>9</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>67.791666666666671</v>
+        <v>54.535087719298247</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,11 +1254,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>24.5</v>
+        <v>33</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>67.791666666666671</v>
+        <v>54.535087719298247</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1289,14 +1289,14 @@
         <v>4.5</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H22">
         <v>4.5</v>
       </c>
       <c r="I22" s="14">
         <f>(F22/G22*100) - F22</f>
-        <v>0</v>
+        <v>0.23684210526315841</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1316,17 +1316,17 @@
         <v>41027</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="G23">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H23">
         <v>1.5</v>
       </c>
       <c r="I23" s="14">
         <f t="shared" ref="I23:I35" si="2">(F23/G23*100) - F23</f>
-        <v>0.125</v>
+        <v>0.1315789473684208</v>
       </c>
       <c r="N23" s="2"/>
     </row>
@@ -1347,17 +1347,17 @@
         <v>41031</v>
       </c>
       <c r="F24">
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H24">
         <v>32.5</v>
       </c>
       <c r="I24" s="14">
         <f t="shared" si="2"/>
-        <v>29.166666666666671</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1377,17 +1377,17 @@
         <v>41036</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H25">
         <v>10</v>
       </c>
       <c r="I25" s="14">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>1.25</v>
       </c>
       <c r="N25" s="2"/>
     </row>
@@ -1408,17 +1408,17 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="G26">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H26">
         <v>30</v>
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>31.166666666666664</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView topLeftCell="Y19" workbookViewId="0">
+      <selection activeCell="AJ41" sqref="AJ41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2015,23 +2015,23 @@
         <v>14</v>
       </c>
       <c r="AC4" s="3">
-        <f>(AC12+AC20+AC28+AC36+AC44+AC52+AC60)</f>
+        <f t="shared" ref="AC4:AG7" si="2">(AC12+AC20+AC28+AC36+AC44+AC52+AC60)</f>
         <v>2</v>
       </c>
       <c r="AD4" s="3">
-        <f>(AD12+AD20+AD28+AD36+AD44+AD52+AD60)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE4" s="3">
-        <f>(AE12+AE20+AE28+AE36+AE44+AE52+AE60)</f>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="3">
-        <f>(AF12+AF20+AF28+AF36+AF44+AF52+AF60)</f>
-        <v>0</v>
-      </c>
-      <c r="AG4" s="3">
-        <f>(AG12+AG20+AG28+AG36+AG44+AG52+AG60)</f>
+      <c r="AE4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH4">
@@ -2041,29 +2041,29 @@
       <c r="AK4" t="s">
         <v>14</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="7">
         <f>SUM(AL12,AL20,AL28,AL36)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM4">
-        <f t="shared" ref="AM4:AQ4" si="2">SUM(AM12,AM20,AM28,AM36)</f>
+        <f t="shared" ref="AM4:AQ4" si="3">SUM(AM12,AM20,AM28,AM36)</f>
         <v>0</v>
       </c>
       <c r="AN4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -2071,23 +2071,23 @@
         <v>17</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:E8" si="3">(B13+B21+B29+B37+B45+B53)</f>
+        <f t="shared" ref="B5:E8" si="4">(B13+B21+B29+B37+B45+B53)</f>
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F7" si="4">(F13+F21+F29+F37+F45)</f>
+        <f t="shared" ref="F5:F7" si="5">(F13+F21+F29+F37+F45)</f>
         <v>0</v>
       </c>
       <c r="G5" s="4">
@@ -2098,23 +2098,23 @@
         <v>17</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:O7" si="5">(K13+K21+K29+K37+K45)</f>
+        <f t="shared" ref="K5:O7" si="6">(K13+K21+K29+K37+K45)</f>
         <v>0</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.6</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P5">
@@ -2125,23 +2125,23 @@
         <v>17</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" ref="T5:X5" si="6">(T13+T21+T29+T37+T45+T53+T61)</f>
+        <f t="shared" ref="T5:X5" si="7">(T13+T21+T29+T37+T45+T53+T61)</f>
         <v>3.5</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="Y5">
@@ -2152,23 +2152,23 @@
         <v>17</v>
       </c>
       <c r="AC5" s="3">
-        <f>(AC13+AC21+AC29+AC37+AC45+AC53+AC61)</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="AD5" s="3">
-        <f>(AD13+AD21+AD29+AD37+AD45+AD53+AD61)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE5" s="3">
-        <f>(AE13+AE21+AE29+AE37+AE45+AE53+AE61)</f>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="3">
-        <f>(AF13+AF21+AF29+AF37+AF45+AF53+AF61)</f>
-        <v>0</v>
-      </c>
-      <c r="AG5" s="3">
-        <f>(AG13+AG21+AG29+AG37+AG45+AG53+AG61)</f>
+      <c r="AE5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH5">
@@ -2180,27 +2180,27 @@
       </c>
       <c r="AL5">
         <f>SUM(AL13,AL21,AL29,AL37)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM5">
-        <f t="shared" ref="AM5:AQ5" si="7">SUM(AM13,AM21,AM29,AM37)</f>
+        <f t="shared" ref="AM5:AQ5" si="8">SUM(AM13,AM21,AM29,AM37)</f>
         <v>0</v>
       </c>
       <c r="AN5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -2208,23 +2208,23 @@
         <v>18</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G6" s="4">
@@ -2235,23 +2235,23 @@
         <v>18</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.1</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P6">
@@ -2262,23 +2262,23 @@
         <v>18</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" ref="T6:X6" si="8">(T14+T22+T30+T38+T46+T54+T62)</f>
+        <f t="shared" ref="T6:X6" si="9">(T14+T22+T30+T38+T46+T54+T62)</f>
         <v>3.5</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="V6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="W6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.5</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Y6">
@@ -2289,23 +2289,23 @@
         <v>18</v>
       </c>
       <c r="AC6" s="3">
-        <f>(AC14+AC22+AC30+AC38+AC46+AC54+AC62)</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="AD6" s="3">
-        <f>(AD14+AD22+AD30+AD38+AD46+AD54+AD62)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE6" s="3">
-        <f>(AE14+AE22+AE30+AE38+AE46+AE54+AE62)</f>
+      <c r="AE6" s="4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF6" s="3">
-        <f>(AF14+AF22+AF30+AF38+AF46+AF54+AF62)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AG6" s="3">
-        <f>(AG14+AG22+AG30+AG38+AG46+AG54+AG62)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AH6">
@@ -2315,29 +2315,29 @@
       <c r="AK6" t="s">
         <v>18</v>
       </c>
-      <c r="AL6">
+      <c r="AL6" s="7">
         <f>SUM(AL22,AL30,AL38,AL14)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM6">
-        <f t="shared" ref="AM6:AQ6" si="9">SUM(AM22,AM30,AM38,AM14)</f>
+        <f t="shared" ref="AM6:AQ6" si="10">SUM(AM22,AM30,AM38,AM14)</f>
         <v>0</v>
       </c>
       <c r="AN6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AO6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AP6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2345,23 +2345,23 @@
         <v>15</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G7" s="4">
@@ -2372,23 +2372,23 @@
         <v>15</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P7">
@@ -2399,23 +2399,23 @@
         <v>15</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" ref="T7:X7" si="10">(T15+T23+T31+T39+T47+T55+T63)</f>
+        <f t="shared" ref="T7:X7" si="11">(T15+T23+T31+T39+T47+T55+T63)</f>
         <v>3.5</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="V7" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="W7" s="3">
-        <f t="shared" si="10"/>
+      <c r="W7" s="4">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5</v>
       </c>
       <c r="Y7">
@@ -2426,23 +2426,23 @@
         <v>15</v>
       </c>
       <c r="AC7" s="3">
-        <f>(AC15+AC23+AC31+AC39+AC47+AC55+AC63)</f>
+        <f t="shared" si="2"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="AD7" s="3">
-        <f>(AD15+AD23+AD31+AD39+AD47+AD55+AD63)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AE7" s="3">
-        <f>(AE15+AE23+AE31+AE39+AE47+AE55+AE63)</f>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3">
-        <f>(AF15+AF23+AF31+AF39+AF47+AF55+AF63)</f>
-        <v>0</v>
-      </c>
-      <c r="AG7" s="3">
-        <f>(AG15+AG23+AG31+AG39+AG47+AG55+AG63)</f>
+      <c r="AE7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH7">
@@ -2454,27 +2454,27 @@
       </c>
       <c r="AL7">
         <f>SUM(AL15,AL23,AL31,AL39)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM7">
-        <f t="shared" ref="AM7:AQ7" si="11">SUM(AM15,AM23,AM31,AM39)</f>
+        <f t="shared" ref="AM7:AQ7" si="12">SUM(AM15,AM23,AM31,AM39)</f>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AO7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AP7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -2482,19 +2482,19 @@
         <v>41</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -2923,8 +2923,8 @@
       <c r="AK14" t="s">
         <v>18</v>
       </c>
-      <c r="AL14">
-        <v>0</v>
+      <c r="AL14" s="7">
+        <v>1</v>
       </c>
       <c r="AM14">
         <v>0</v>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="AQ14">
         <f>SUM(AL14:AP14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AQ16" s="12">
         <f>SUM(AQ12:AQ15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:43">
@@ -4379,8 +4379,8 @@
       <c r="AK36" t="s">
         <v>14</v>
       </c>
-      <c r="AL36">
-        <v>0</v>
+      <c r="AL36" s="7">
+        <v>2</v>
       </c>
       <c r="AM36">
         <v>0</v>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="AQ36">
         <f>SUM(AL36:AP36)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:43">
@@ -4479,8 +4479,8 @@
       <c r="AK37" t="s">
         <v>17</v>
       </c>
-      <c r="AL37">
-        <v>0</v>
+      <c r="AL37" s="7">
+        <v>3</v>
       </c>
       <c r="AM37">
         <v>0</v>
@@ -4496,7 +4496,7 @@
       </c>
       <c r="AQ37">
         <f>SUM(AL37:AP37)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:43">
@@ -4575,8 +4575,8 @@
       <c r="AK38" t="s">
         <v>18</v>
       </c>
-      <c r="AL38">
-        <v>0</v>
+      <c r="AL38" s="7">
+        <v>3</v>
       </c>
       <c r="AM38">
         <v>0</v>
@@ -4592,7 +4592,7 @@
       </c>
       <c r="AQ38">
         <f>SUM(AL38:AP38)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -4671,8 +4671,8 @@
       <c r="AK39" t="s">
         <v>15</v>
       </c>
-      <c r="AL39">
-        <v>0</v>
+      <c r="AL39" s="7">
+        <v>3</v>
       </c>
       <c r="AM39">
         <v>0</v>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="AQ39">
         <f>SUM(AL39:AP39)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:43">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="AQ40" s="12">
         <f>SUM(AQ36:AQ39)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:43">
@@ -5541,8 +5541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P21" sqref="A1:P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
worked with the different gameObjects
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G31:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>9</v>
+        <v>9.125</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>54.535087719298247</v>
+        <v>53.368421052631575</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,11 +1254,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>33</v>
+        <v>33.5</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>54.535087719298247</v>
+        <v>53.368421052631575</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1408,17 +1408,17 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
       <c r="G26">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H26">
         <v>30</v>
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>31.166666666666664</v>
+        <v>30</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView topLeftCell="Y19" workbookViewId="0">
-      <selection activeCell="AJ41" sqref="AJ41"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AK9" sqref="AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2319,9 +2319,9 @@
         <f>SUM(AL22,AL30,AL38,AL14)</f>
         <v>4</v>
       </c>
-      <c r="AM6">
+      <c r="AM6" s="7">
         <f t="shared" ref="AM6:AQ6" si="10">SUM(AM22,AM30,AM38,AM14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN6">
         <f t="shared" si="10"/>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="AQ6">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -4578,8 +4578,8 @@
       <c r="AL38" s="7">
         <v>3</v>
       </c>
-      <c r="AM38">
-        <v>0</v>
+      <c r="AM38" s="7">
+        <v>2</v>
       </c>
       <c r="AN38">
         <v>0</v>
@@ -4592,7 +4592,7 @@
       </c>
       <c r="AQ38">
         <f>SUM(AL38:AP38)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="AQ40" s="12">
         <f>SUM(AQ36:AQ39)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:43">
@@ -5541,7 +5541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor change in WorldHandler and GameScreen
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>59.5</v>
+        <v>60.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>21.824999999999999</v>
+        <v>31.824999999999999</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>33.489974937343355</v>
+        <v>32.966165413533837</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1624,11 +1624,11 @@
       </c>
       <c r="F33" s="7">
         <f>SUM(F34:F35)</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G33" s="7">
         <f>SUM(G34:G35)</f>
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="H33" s="7">
         <f>(SUM(H34:H35))</f>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="I33" s="16">
         <f>I34+I35</f>
-        <v>1.1666666666666667</v>
+        <v>0.64285714285714279</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1653,17 +1653,17 @@
         <v>41036</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G34">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H34">
         <v>4</v>
       </c>
       <c r="I34" s="14">
         <f t="shared" si="2"/>
-        <v>1.1666666666666667</v>
+        <v>0.64285714285714279</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="AO6" s="7">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AP6">
         <f t="shared" si="10"/>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="AQ6">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>38.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -2932,15 +2932,15 @@
       <c r="AN14">
         <v>0</v>
       </c>
-      <c r="AO14">
-        <v>0</v>
+      <c r="AO14" s="7">
+        <v>1</v>
       </c>
       <c r="AP14">
         <v>0</v>
       </c>
       <c r="AQ14">
         <f>SUM(AL14:AP14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AQ16" s="12">
         <f>SUM(AQ12:AQ15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:43">

</xml_diff>

<commit_message>
more minor fixes in WorldHandler
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>60.5</v>
+        <v>61.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>32.966165413533837</v>
+        <v>33.680451127819545</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>59</v>
+        <v>59.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>32.323308270676691</v>
+        <v>32.823308270676691</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1408,7 +1408,7 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="G26">
         <v>50</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="F33" s="7">
         <f>SUM(F34:F35)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G33" s="7">
         <f>SUM(G34:G35)</f>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="I33" s="16">
         <f>I34+I35</f>
-        <v>0.64285714285714279</v>
+        <v>0.85714285714285721</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1653,7 +1653,7 @@
         <v>41036</v>
       </c>
       <c r="F34">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G34">
         <v>70</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="I34" s="14">
         <f t="shared" si="2"/>
-        <v>0.64285714285714279</v>
+        <v>0.85714285714285721</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AN44" sqref="AN44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="AO6" s="7">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="AP6">
         <f t="shared" si="10"/>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="AQ6">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>39.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -4585,14 +4585,14 @@
         <v>3</v>
       </c>
       <c r="AO38" s="7">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AP38">
         <v>0</v>
       </c>
       <c r="AQ38">
         <f>SUM(AL38:AP38)</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="AQ40" s="12">
         <f>SUM(AQ36:AQ39)</f>
-        <v>37.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:43">

</xml_diff>

<commit_message>
minor fixes in camera and worldhandler
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>61.5</v>
+        <v>78.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>31.824999999999999</v>
+        <v>32.325000000000003</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>33.680451127819545</v>
+        <v>42.109022556390975</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,11 +1254,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>59.5</v>
+        <v>76.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>55.3</v>
+        <v>57.3</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>32.823308270676691</v>
+        <v>41.251879699248121</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1408,7 +1408,7 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G26">
         <v>50</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1469,17 +1469,17 @@
         <v>41036</v>
       </c>
       <c r="F28">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G28">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="H28">
         <v>20</v>
       </c>
       <c r="I28" s="14">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>6.428571428571427</v>
       </c>
       <c r="N28" s="2"/>
     </row>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:AQ64"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AN44" sqref="AN44"/>
+      <selection activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2057,13 +2057,13 @@
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -2194,13 +2194,13 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -2331,13 +2331,13 @@
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" s="7">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="10"/>
-        <v>13.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2468,13 +2468,13 @@
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" s="7">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="12"/>
-        <v>9</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -4391,12 +4391,12 @@
       <c r="AO36" s="7">
         <v>2.5</v>
       </c>
-      <c r="AP36">
-        <v>0</v>
+      <c r="AP36" s="7">
+        <v>4.5</v>
       </c>
       <c r="AQ36">
         <f>SUM(AL36:AP36)</f>
-        <v>7.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:43">
@@ -4491,12 +4491,12 @@
       <c r="AO37" s="7">
         <v>3</v>
       </c>
-      <c r="AP37">
-        <v>0</v>
+      <c r="AP37" s="7">
+        <v>4.5</v>
       </c>
       <c r="AQ37">
         <f>SUM(AL37:AP37)</f>
-        <v>10</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="38" spans="1:43">
@@ -4587,12 +4587,12 @@
       <c r="AO38" s="7">
         <v>3.5</v>
       </c>
-      <c r="AP38">
-        <v>0</v>
+      <c r="AP38" s="7">
+        <v>4.5</v>
       </c>
       <c r="AQ38">
         <f>SUM(AL38:AP38)</f>
-        <v>11.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -4683,12 +4683,12 @@
       <c r="AO39" s="7">
         <v>3</v>
       </c>
-      <c r="AP39">
-        <v>0</v>
+      <c r="AP39" s="7">
+        <v>3.5</v>
       </c>
       <c r="AQ39">
         <f>SUM(AL39:AP39)</f>
-        <v>9</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="40" spans="1:43">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="AQ40" s="12">
         <f>SUM(AQ36:AQ39)</f>
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:43">

</xml_diff>

<commit_message>
fixed the rendering problem
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>78.5</v>
+        <v>80</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>32.325000000000003</v>
+        <v>39.825000000000003</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>42.109022556390975</v>
+        <v>42.251879699248121</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>76.5</v>
+        <v>77.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>41.251879699248121</v>
+        <v>42.251879699248121</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1408,7 +1408,7 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G26">
         <v>50</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1624,11 +1624,11 @@
       </c>
       <c r="F33" s="7">
         <f>SUM(F34:F35)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G33" s="7">
         <f>SUM(G34:G35)</f>
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="H33" s="7">
         <f>(SUM(H34:H35))</f>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="I33" s="16">
         <f>I34+I35</f>
-        <v>0.85714285714285721</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1653,17 +1653,17 @@
         <v>41036</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H34">
         <v>4</v>
       </c>
       <c r="I34" s="14">
         <f t="shared" si="2"/>
-        <v>0.85714285714285721</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:AQ64"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9"/>
+      <selection activeCell="AN17" sqref="AN17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2333,11 +2333,11 @@
       </c>
       <c r="AP6" s="7">
         <f t="shared" si="10"/>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="AQ8" s="12">
         <f>SUM(AQ4:AQ7)</f>
-        <v>57</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -2935,12 +2935,12 @@
       <c r="AO14" s="7">
         <v>1</v>
       </c>
-      <c r="AP14">
-        <v>0</v>
+      <c r="AP14" s="7">
+        <v>0.5</v>
       </c>
       <c r="AQ14">
         <f>SUM(AL14:AP14)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AQ16" s="12">
         <f>SUM(AQ12:AQ15)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:43">
@@ -4588,11 +4588,11 @@
         <v>3.5</v>
       </c>
       <c r="AP38" s="7">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="AQ38">
         <f>SUM(AL38:AP38)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="AQ40" s="12">
         <f>SUM(AQ36:AQ39)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:43">
@@ -5542,7 +5542,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fixed error with heap corruption, added work time and R7
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="107">
   <si>
     <t>L1</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>Progammering</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -722,7 +728,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,11 +1229,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>82.5</v>
+        <v>93.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>27.2</v>
+        <v>27.324999999999999</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1235,7 +1241,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>42.251879699248121</v>
+        <v>42.409774436090231</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1254,11 +1260,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>77.5</v>
+        <v>86.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>57.3</v>
+        <v>57.8</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1266,7 +1272,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>42.251879699248121</v>
+        <v>42.409774436090231</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1316,7 +1322,7 @@
         <v>41027</v>
       </c>
       <c r="F23">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="G23">
         <v>95</v>
@@ -1326,7 +1332,7 @@
       </c>
       <c r="I23" s="14">
         <f t="shared" ref="I23:I35" si="2">(F23/G23*100) - F23</f>
-        <v>0.23684210526315841</v>
+        <v>0.39473684210526283</v>
       </c>
       <c r="N23" s="2"/>
     </row>
@@ -1408,10 +1414,10 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H26">
         <v>30</v>
@@ -1729,7 +1735,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -1764,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ64"/>
+  <dimension ref="A1:AZ64"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AO9" sqref="AO9"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AR15" sqref="AR15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1805,7 +1811,7 @@
     <col min="43" max="43" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:52">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1836,8 +1842,14 @@
       <c r="AL1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:43">
+      <c r="AT1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -1853,8 +1865,11 @@
       <c r="AM2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:43">
+      <c r="AV2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -1930,8 +1945,23 @@
       <c r="AP3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:43">
+      <c r="AU3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2067,8 +2097,35 @@
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:43">
+      <c r="AT4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU4" s="7">
+        <f>SUM(AU12,AU20,AU28,AU36)</f>
+        <v>3</v>
+      </c>
+      <c r="AV4" s="5">
+        <f>SUM(AV12,AV20,AV28,AV36)</f>
+        <v>0</v>
+      </c>
+      <c r="AW4" s="5">
+        <f>SUM(AW12,AW20,AW28,AW36)</f>
+        <v>0</v>
+      </c>
+      <c r="AX4" s="5">
+        <f>SUM(AX12,AX20,AX28,AX36)</f>
+        <v>0</v>
+      </c>
+      <c r="AY4" s="5">
+        <f>SUM(AY12,AY20,AY28,AY36)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <f>SUM(AU4:AY4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2204,8 +2261,35 @@
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:43">
+      <c r="AT5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU5" s="7">
+        <f>SUM(AU13,AU21,AU29,AU37)</f>
+        <v>3</v>
+      </c>
+      <c r="AV5" s="5">
+        <f>SUM(AV13,AV21,AV29,AV37)</f>
+        <v>0</v>
+      </c>
+      <c r="AW5" s="5">
+        <f>SUM(AW13,AW21,AW29,AW37)</f>
+        <v>0</v>
+      </c>
+      <c r="AX5" s="5">
+        <f>SUM(AX13,AX21,AX29,AX37)</f>
+        <v>0</v>
+      </c>
+      <c r="AY5" s="5">
+        <f>SUM(AY13,AY21,AY29,AY37)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <f>SUM(AU5:AY5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2341,8 +2425,35 @@
         <f t="shared" si="10"/>
         <v>20.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:43">
+      <c r="AT6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU6" s="7">
+        <f>SUM(AU22,AU30,AU38,AU14)</f>
+        <v>4</v>
+      </c>
+      <c r="AV6" s="5">
+        <f>SUM(AV22,AV30,AV38,AV14)</f>
+        <v>0</v>
+      </c>
+      <c r="AW6" s="5">
+        <f>SUM(AW22,AW30,AW38,AW14)</f>
+        <v>0</v>
+      </c>
+      <c r="AX6" s="5">
+        <f>SUM(AX22,AX30,AX38,AX14)</f>
+        <v>0</v>
+      </c>
+      <c r="AY6" s="5">
+        <f>SUM(AY22,AY30,AY38,AY14)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <f>SUM(AU6:AY6)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2478,8 +2589,35 @@
         <f t="shared" si="12"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:43">
+      <c r="AT7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU7" s="7">
+        <f>SUM(AU15,AU23,AU31,AU39)</f>
+        <v>2</v>
+      </c>
+      <c r="AV7" s="5">
+        <f>SUM(AV15,AV23,AV31,AV39)</f>
+        <v>0</v>
+      </c>
+      <c r="AW7" s="5">
+        <f>SUM(AW15,AW23,AW31,AW39)</f>
+        <v>0</v>
+      </c>
+      <c r="AX7" s="5">
+        <f>SUM(AX15,AX23,AX31,AX39)</f>
+        <v>0</v>
+      </c>
+      <c r="AY7" s="5">
+        <f>SUM(AY15,AY23,AY31,AY39)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <f>SUM(AU7:AY7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -2538,14 +2676,18 @@
         <f>SUM(AQ4:AQ7)</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:43">
+      <c r="AZ8" s="12">
+        <f t="shared" ref="AZ8" si="13">SUM(AZ4:AZ7)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52">
       <c r="G9" s="11">
         <f>SUM(G4:G8)</f>
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:52">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -2562,8 +2704,11 @@
       <c r="AM10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:43">
+      <c r="AV10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>36</v>
@@ -2641,8 +2786,23 @@
       <c r="AP11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:43">
+      <c r="AU11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2741,8 +2901,30 @@
         <f>SUM(AL12:AP12)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:43">
+      <c r="AT12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" ref="AZ12:AZ15" si="14">SUM(AU12:AY12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2841,8 +3023,30 @@
         <f>SUM(AL13:AP13)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:43">
+      <c r="AT13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ13">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2944,8 +3148,30 @@
         <f>SUM(AL14:AP14)</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:43">
+      <c r="AT14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -3044,8 +3270,30 @@
         <f>SUM(AL15:AP15)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:43">
+      <c r="AT15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -3097,8 +3345,12 @@
         <f>SUM(AQ12:AQ15)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:43">
+      <c r="AZ16" s="12">
+        <f t="shared" ref="AZ16" si="15">SUM(AZ12:AZ15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3110,7 +3362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:52">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -3132,8 +3384,11 @@
       <c r="AM18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:43">
+      <c r="AV18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -3211,8 +3466,23 @@
       <c r="AP19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:43">
+      <c r="AU19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
@@ -3306,8 +3576,30 @@
         <f>SUM(AL20:AP20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:43">
+      <c r="AT20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU20">
+        <v>0</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+      <c r="AW20">
+        <v>0</v>
+      </c>
+      <c r="AX20">
+        <v>0</v>
+      </c>
+      <c r="AY20">
+        <v>0</v>
+      </c>
+      <c r="AZ20">
+        <f t="shared" ref="AZ20:AZ23" si="16">SUM(AU20:AY20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:52">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -3401,8 +3693,30 @@
         <f>SUM(AL21:AP21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:43">
+      <c r="AT21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU21">
+        <v>0</v>
+      </c>
+      <c r="AV21">
+        <v>0</v>
+      </c>
+      <c r="AW21">
+        <v>0</v>
+      </c>
+      <c r="AX21">
+        <v>0</v>
+      </c>
+      <c r="AY21">
+        <v>0</v>
+      </c>
+      <c r="AZ21">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:52">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
@@ -3496,8 +3810,30 @@
         <f>SUM(AL22:AP22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:43">
+      <c r="AT22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU22">
+        <v>0</v>
+      </c>
+      <c r="AV22">
+        <v>0</v>
+      </c>
+      <c r="AW22">
+        <v>0</v>
+      </c>
+      <c r="AX22">
+        <v>0</v>
+      </c>
+      <c r="AY22">
+        <v>0</v>
+      </c>
+      <c r="AZ22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:52">
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
@@ -3591,8 +3927,30 @@
         <f>SUM(AL23:AP23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:43">
+      <c r="AT23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>0</v>
+      </c>
+      <c r="AW23">
+        <v>0</v>
+      </c>
+      <c r="AX23">
+        <v>0</v>
+      </c>
+      <c r="AY23">
+        <v>0</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:52">
       <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
@@ -3646,8 +4004,12 @@
         <f>SUM(AQ20:AQ23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:43">
+      <c r="AZ24" s="12">
+        <f t="shared" ref="AZ24" si="17">SUM(AZ20:AZ23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:52">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3659,7 +4021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:52">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -3681,8 +4043,11 @@
       <c r="AM26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:43">
+      <c r="AV26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:52">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>36</v>
@@ -3760,8 +4125,23 @@
       <c r="AP27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:43">
+      <c r="AU27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX27" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:52">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -3858,8 +4238,30 @@
         <f>SUM(AL28:AP28)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:43">
+      <c r="AT28" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU28">
+        <v>0</v>
+      </c>
+      <c r="AV28">
+        <v>0</v>
+      </c>
+      <c r="AW28">
+        <v>0</v>
+      </c>
+      <c r="AX28">
+        <v>0</v>
+      </c>
+      <c r="AY28">
+        <v>0</v>
+      </c>
+      <c r="AZ28">
+        <f t="shared" ref="AZ28:AZ31" si="18">SUM(AU28:AY28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:52">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -3949,8 +4351,30 @@
         <f>SUM(AL29:AP29)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:43">
+      <c r="AT29" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU29">
+        <v>0</v>
+      </c>
+      <c r="AV29">
+        <v>0</v>
+      </c>
+      <c r="AW29">
+        <v>0</v>
+      </c>
+      <c r="AX29">
+        <v>0</v>
+      </c>
+      <c r="AY29">
+        <v>0</v>
+      </c>
+      <c r="AZ29">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:52">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -4040,8 +4464,30 @@
         <f>SUM(AL30:AP30)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:43">
+      <c r="AT30" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU30">
+        <v>0</v>
+      </c>
+      <c r="AV30">
+        <v>0</v>
+      </c>
+      <c r="AW30">
+        <v>0</v>
+      </c>
+      <c r="AX30">
+        <v>0</v>
+      </c>
+      <c r="AY30">
+        <v>0</v>
+      </c>
+      <c r="AZ30">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:52">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
@@ -4135,8 +4581,30 @@
         <f>SUM(AL31:AP31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:43">
+      <c r="AT31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU31">
+        <v>0</v>
+      </c>
+      <c r="AV31">
+        <v>0</v>
+      </c>
+      <c r="AW31">
+        <v>0</v>
+      </c>
+      <c r="AX31">
+        <v>0</v>
+      </c>
+      <c r="AY31">
+        <v>0</v>
+      </c>
+      <c r="AZ31">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:52">
       <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
@@ -4190,8 +4658,12 @@
         <f>SUM(AQ28:AQ31)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:43">
+      <c r="AZ32" s="12">
+        <f t="shared" ref="AZ32" si="19">SUM(AZ28:AZ31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:52">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -4203,7 +4675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:52">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -4222,11 +4694,20 @@
       <c r="AD34" t="s">
         <v>5</v>
       </c>
+      <c r="AK34" t="s">
+        <v>106</v>
+      </c>
       <c r="AM34" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:43">
+      <c r="AT34" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:52">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
@@ -4304,8 +4785,23 @@
       <c r="AP35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:43">
+      <c r="AU35" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX35" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:52">
       <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
@@ -4400,8 +4896,30 @@
         <f>SUM(AL36:AP36)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:43">
+      <c r="AT36" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU36" s="7">
+        <v>3</v>
+      </c>
+      <c r="AV36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ36">
+        <f t="shared" ref="AZ36:AZ39" si="20">SUM(AU36:AY36)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:52">
       <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
@@ -4500,8 +5018,30 @@
         <f>SUM(AL37:AP37)</f>
         <v>14.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:43">
+      <c r="AT37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU37" s="7">
+        <v>3</v>
+      </c>
+      <c r="AV37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ37">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:52">
       <c r="A38" s="5" t="s">
         <v>18</v>
       </c>
@@ -4596,8 +5136,30 @@
         <f>SUM(AL38:AP38)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:43">
+      <c r="AT38" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU38" s="7">
+        <v>4</v>
+      </c>
+      <c r="AV38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ38">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:52">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -4692,8 +5254,30 @@
         <f>SUM(AL39:AP39)</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:43">
+      <c r="AT39" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU39" s="7">
+        <v>2</v>
+      </c>
+      <c r="AV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ39">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:52">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -4740,8 +5324,12 @@
         <f>SUM(AQ36:AQ39)</f>
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:43">
+      <c r="AZ40" s="12">
+        <f t="shared" ref="AZ40" si="21">SUM(AZ36:AZ39)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:52">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -4753,7 +5341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:43">
+    <row r="42" spans="1:52">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -4773,7 +5361,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:52">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>36</v>
@@ -4837,7 +5425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:52">
       <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
@@ -4908,7 +5496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:43">
+    <row r="45" spans="1:52">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -4979,7 +5567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:52">
       <c r="A46" s="5" t="s">
         <v>18</v>
       </c>
@@ -5050,7 +5638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:52">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -5121,7 +5709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:52">
       <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
@@ -5188,6 +5776,11 @@
       <c r="AD50" t="s">
         <v>44</v>
       </c>
+      <c r="AL50" s="5"/>
+      <c r="AM50" s="5"/>
+      <c r="AN50" s="5"/>
+      <c r="AO50" s="5"/>
+      <c r="AP50" s="5"/>
     </row>
     <row r="51" spans="1:42">
       <c r="A51" s="5"/>
@@ -5543,7 +6136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor fixed in GameScreen
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1229,11 +1229,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>105.5</v>
+        <v>117.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>27.65</v>
+        <v>29.524999999999999</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>60.332978167343505</v>
+        <v>42.772372106737436</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1260,11 +1260,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>98.5</v>
+        <v>110.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>59.1</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>60.332978167343505</v>
+        <v>42.772372106737436</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1414,17 +1414,17 @@
         <v>41036</v>
       </c>
       <c r="F26">
-        <v>34.5</v>
+        <v>39.5</v>
       </c>
       <c r="G26">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="H26">
         <v>30</v>
       </c>
       <c r="I26" s="14">
         <f t="shared" si="2"/>
-        <v>28.227272727272734</v>
+        <v>13.166666666666664</v>
       </c>
       <c r="N26" s="2"/>
     </row>
@@ -1506,17 +1506,17 @@
         <v>41036</v>
       </c>
       <c r="F29">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H29">
         <v>25</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="N29" s="2"/>
     </row>
@@ -1568,17 +1568,17 @@
         <v>41043</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H31">
         <v>15</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" si="2"/>
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="N31" s="2"/>
     </row>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:AZ64"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AL35" sqref="AL35:AP39"/>
+      <selection activeCell="AS10" sqref="AS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2108,9 +2108,9 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="AW4" s="5">
+      <c r="AW4" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AX4" s="5">
         <f t="shared" si="4"/>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="AZ4">
         <f>SUM(AU4:AY4)</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -2272,9 +2272,9 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="AW5" s="5">
+      <c r="AW5" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AX5" s="5">
         <f t="shared" si="4"/>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="AZ5">
         <f>SUM(AU5:AY5)</f>
-        <v>9</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:52">
@@ -2432,13 +2432,13 @@
         <f>SUM(AU22,AU30,AU38,AU14)</f>
         <v>4</v>
       </c>
-      <c r="AV6" s="5">
+      <c r="AV6" s="7">
         <f>SUM(AV22,AV30,AV38,AV14)</f>
-        <v>0</v>
-      </c>
-      <c r="AW6" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW6" s="7">
         <f>SUM(AW22,AW30,AW38,AW14)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AX6" s="5">
         <f>SUM(AX22,AX30,AX38,AX14)</f>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="AZ6">
         <f>SUM(AU6:AY6)</f>
-        <v>4</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -2600,9 +2600,9 @@
         <f>SUM(AV15,AV23,AV31,AV39)</f>
         <v>3</v>
       </c>
-      <c r="AW7" s="5">
+      <c r="AW7" s="7">
         <f>SUM(AW15,AW23,AW31,AW39)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AX7" s="5">
         <f>SUM(AX15,AX23,AX31,AX39)</f>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="AZ7">
         <f>SUM(AU7:AY7)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="8" spans="1:52">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="AZ8" s="12">
         <f t="shared" ref="AZ8" si="14">SUM(AZ4:AZ7)</f>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -4905,8 +4905,8 @@
       <c r="AV36" s="7">
         <v>3</v>
       </c>
-      <c r="AW36" s="5">
-        <v>0</v>
+      <c r="AW36" s="7">
+        <v>0.5</v>
       </c>
       <c r="AX36" s="5">
         <v>0</v>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="AZ36">
         <f t="shared" ref="AZ36:AZ39" si="21">SUM(AU36:AY36)</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="37" spans="1:52">
@@ -5027,8 +5027,8 @@
       <c r="AV37" s="7">
         <v>6</v>
       </c>
-      <c r="AW37" s="5">
-        <v>0</v>
+      <c r="AW37" s="7">
+        <v>2.5</v>
       </c>
       <c r="AX37" s="5">
         <v>0</v>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="AZ37">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="38" spans="1:52">
@@ -5142,9 +5142,11 @@
       <c r="AU38" s="7">
         <v>4</v>
       </c>
-      <c r="AV38" s="5"/>
-      <c r="AW38" s="5">
-        <v>0</v>
+      <c r="AV38" s="7">
+        <v>5</v>
+      </c>
+      <c r="AW38" s="7">
+        <v>2.5</v>
       </c>
       <c r="AX38" s="5">
         <v>0</v>
@@ -5154,7 +5156,7 @@
       </c>
       <c r="AZ38">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="39" spans="1:52">
@@ -5261,8 +5263,8 @@
       <c r="AV39" s="7">
         <v>3</v>
       </c>
-      <c r="AW39" s="5">
-        <v>0</v>
+      <c r="AW39" s="7">
+        <v>2.5</v>
       </c>
       <c r="AX39" s="5">
         <v>0</v>
@@ -5272,7 +5274,7 @@
       </c>
       <c r="AZ39">
         <f t="shared" si="21"/>
-        <v>5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="40" spans="1:52">
@@ -5324,7 +5326,7 @@
       </c>
       <c r="AZ40" s="12">
         <f t="shared" ref="AZ40" si="22">SUM(AZ36:AZ39)</f>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:52">

</xml_diff>

<commit_message>
graphics and finished the demo
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1229,19 +1229,19 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>117.5</v>
+        <v>128.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>29.524999999999999</v>
+        <v>56.774999999999999</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
-        <v>170.5</v>
+        <v>166.5</v>
       </c>
       <c r="I20" s="14">
         <f>I21+I32+I33+I36+I37+I38</f>
-        <v>42.772372106737436</v>
+        <v>25.858395989974934</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1260,11 +1260,11 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(F22:F31)</f>
-        <v>110.5</v>
+        <v>119.5</v>
       </c>
       <c r="G21" s="7">
         <f>SUM(G22:G31)/10</f>
-        <v>66.599999999999994</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="H21" s="7">
         <f>SUM(H22:H31)</f>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="I21" s="16">
         <f>(SUM(I22:I31))</f>
-        <v>42.772372106737436</v>
+        <v>25.858395989974934</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1325,14 +1325,14 @@
         <v>9</v>
       </c>
       <c r="G23">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="H23">
         <v>1.5</v>
       </c>
       <c r="I23" s="14">
         <f t="shared" ref="I23:I35" si="2">(F23/G23*100) - F23</f>
-        <v>6</v>
+        <v>0.47368421052631682</v>
       </c>
       <c r="N23" s="2"/>
     </row>
@@ -1356,14 +1356,14 @@
         <v>22.5</v>
       </c>
       <c r="G24">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H24">
         <v>32.5</v>
       </c>
       <c r="I24" s="14">
         <f t="shared" si="2"/>
-        <v>9.6428571428571459</v>
+        <v>1.1842105263157876</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1478,14 +1478,14 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H28">
         <v>20</v>
       </c>
       <c r="I28" s="14">
         <f t="shared" si="2"/>
-        <v>2.647058823529413</v>
+        <v>0.78947368421052566</v>
       </c>
       <c r="N28" s="2"/>
     </row>
@@ -1509,14 +1509,14 @@
         <v>3</v>
       </c>
       <c r="G29">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H29">
         <v>25</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="N29" s="2"/>
     </row>
@@ -1568,17 +1568,17 @@
         <v>41043</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G31">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="H31">
         <v>15</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>6.428571428571427</v>
       </c>
       <c r="N31" s="2"/>
     </row>
@@ -1599,10 +1599,10 @@
         <v>41043</v>
       </c>
       <c r="F32" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H32" s="7">
         <v>4</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I36" s="7"/>
     </row>
@@ -1737,7 +1737,9 @@
       <c r="F37" s="7">
         <v>2</v>
       </c>
-      <c r="G37" s="7"/>
+      <c r="G37" s="7">
+        <v>100</v>
+      </c>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
     </row>
@@ -1773,7 +1775,7 @@
   <dimension ref="A1:AZ64"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AS10" sqref="AS10"/>
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2112,9 +2114,9 @@
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="AX4" s="5">
+      <c r="AX4" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY4" s="5">
         <f t="shared" si="4"/>
@@ -2122,7 +2124,7 @@
       </c>
       <c r="AZ4">
         <f>SUM(AU4:AY4)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -2440,9 +2442,9 @@
         <f>SUM(AW22,AW30,AW38,AW14)</f>
         <v>2.5</v>
       </c>
-      <c r="AX6" s="5">
+      <c r="AX6" s="7">
         <f>SUM(AX22,AX30,AX38,AX14)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AY6" s="5">
         <f>SUM(AY22,AY30,AY38,AY14)</f>
@@ -2450,7 +2452,7 @@
       </c>
       <c r="AZ6">
         <f>SUM(AU6:AY6)</f>
-        <v>11.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -2604,9 +2606,9 @@
         <f>SUM(AW15,AW23,AW31,AW39)</f>
         <v>2.5</v>
       </c>
-      <c r="AX7" s="5">
+      <c r="AX7" s="7">
         <f>SUM(AX15,AX23,AX31,AX39)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AY7" s="5">
         <f>SUM(AY15,AY23,AY31,AY39)</f>
@@ -2614,7 +2616,7 @@
       </c>
       <c r="AZ7">
         <f>SUM(AU7:AY7)</f>
-        <v>7.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:52">
@@ -2678,7 +2680,7 @@
       </c>
       <c r="AZ8" s="12">
         <f t="shared" ref="AZ8" si="14">SUM(AZ4:AZ7)</f>
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -4908,15 +4910,15 @@
       <c r="AW36" s="7">
         <v>0.5</v>
       </c>
-      <c r="AX36" s="5">
-        <v>0</v>
+      <c r="AX36" s="7">
+        <v>2</v>
       </c>
       <c r="AY36" s="5">
         <v>0</v>
       </c>
       <c r="AZ36">
         <f t="shared" ref="AZ36:AZ39" si="21">SUM(AU36:AY36)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="37" spans="1:52">
@@ -5148,15 +5150,15 @@
       <c r="AW38" s="7">
         <v>2.5</v>
       </c>
-      <c r="AX38" s="5">
-        <v>0</v>
+      <c r="AX38" s="7">
+        <v>3.5</v>
       </c>
       <c r="AY38" s="5">
         <v>0</v>
       </c>
       <c r="AZ38">
         <f t="shared" si="21"/>
-        <v>11.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:52">
@@ -5266,15 +5268,15 @@
       <c r="AW39" s="7">
         <v>2.5</v>
       </c>
-      <c r="AX39" s="5">
-        <v>0</v>
+      <c r="AX39" s="7">
+        <v>3.5</v>
       </c>
       <c r="AY39" s="5">
         <v>0</v>
       </c>
       <c r="AZ39">
         <f t="shared" si="21"/>
-        <v>7.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:52">
@@ -5326,7 +5328,7 @@
       </c>
       <c r="AZ40" s="12">
         <f t="shared" ref="AZ40" si="22">SUM(AZ36:AZ39)</f>
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:52">
@@ -6136,7 +6138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished L3 as well as the R7
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I38" sqref="A19:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1229,11 +1229,11 @@
       </c>
       <c r="F20">
         <f>F21+F32+F33+F36+F37+F38</f>
-        <v>128.5</v>
+        <v>131.5</v>
       </c>
       <c r="G20" s="14">
         <f>(G21+G32+G33+G36)/4</f>
-        <v>56.774999999999999</v>
+        <v>94.15</v>
       </c>
       <c r="H20">
         <f>H21+H32+H33+H36+H37+H38</f>
@@ -1331,7 +1331,7 @@
         <v>1.5</v>
       </c>
       <c r="I23" s="14">
-        <f t="shared" ref="I23:I35" si="2">(F23/G23*100) - F23</f>
+        <f t="shared" ref="I23:I36" si="2">(F23/G23*100) - F23</f>
         <v>0.47368421052631682</v>
       </c>
       <c r="N23" s="2"/>
@@ -1630,11 +1630,11 @@
       </c>
       <c r="F33" s="7">
         <f>SUM(F34:F35)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G33" s="7">
         <f>SUM(G34:G35)/2</f>
-        <v>50.5</v>
+        <v>100</v>
       </c>
       <c r="H33" s="7">
         <f>(SUM(H34:H35))</f>
@@ -1686,10 +1686,10 @@
         <v>41043</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H35">
         <v>4</v>
@@ -1716,13 +1716,18 @@
         <v>41043</v>
       </c>
       <c r="F36" s="7">
-        <v>0</v>
-      </c>
-      <c r="G36" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G36" s="7">
+        <v>100</v>
+      </c>
       <c r="H36" s="7">
         <v>0</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="7" t="s">
@@ -1775,7 +1780,7 @@
   <dimension ref="A1:AZ64"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="BB12" sqref="BB12"/>
+      <selection activeCell="AZ40" sqref="AT1:AZ40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2444,15 +2449,15 @@
       </c>
       <c r="AX6" s="7">
         <f>SUM(AX22,AX30,AX38,AX14)</f>
-        <v>3.5</v>
-      </c>
-      <c r="AY6" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="AY6" s="7">
         <f>SUM(AY22,AY30,AY38,AY14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ6">
         <f>SUM(AU6:AY6)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -2680,7 +2685,7 @@
       </c>
       <c r="AZ8" s="12">
         <f t="shared" ref="AZ8" si="14">SUM(AZ4:AZ7)</f>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -3162,15 +3167,15 @@
       <c r="AW14" s="5">
         <v>0</v>
       </c>
-      <c r="AX14" s="5">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="5">
-        <v>0</v>
+      <c r="AX14" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY14" s="7">
+        <v>1</v>
       </c>
       <c r="AZ14">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:52">
@@ -3349,7 +3354,7 @@
       </c>
       <c r="AZ16" s="12">
         <f t="shared" ref="AZ16" si="16">SUM(AZ12:AZ15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:52">
@@ -3827,12 +3832,12 @@
       <c r="AX22">
         <v>0</v>
       </c>
-      <c r="AY22">
-        <v>0</v>
+      <c r="AY22" s="7">
+        <v>1</v>
       </c>
       <c r="AZ22">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:52">
@@ -4008,7 +4013,7 @@
       </c>
       <c r="AZ24" s="12">
         <f t="shared" ref="AZ24" si="18">SUM(AZ20:AZ23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:52">
@@ -4478,15 +4483,15 @@
       <c r="AW30">
         <v>0</v>
       </c>
-      <c r="AX30">
-        <v>0</v>
+      <c r="AX30" s="7">
+        <v>1</v>
       </c>
       <c r="AY30">
         <v>0</v>
       </c>
       <c r="AZ30">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:52">
@@ -4595,15 +4600,15 @@
       <c r="AW31">
         <v>0</v>
       </c>
-      <c r="AX31">
-        <v>0</v>
+      <c r="AX31" s="7">
+        <v>1</v>
       </c>
       <c r="AY31">
         <v>0</v>
       </c>
       <c r="AZ31">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:52">
@@ -4662,7 +4667,7 @@
       </c>
       <c r="AZ32" s="12">
         <f t="shared" ref="AZ32" si="20">SUM(AZ28:AZ31)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:52">
@@ -5151,14 +5156,14 @@
         <v>2.5</v>
       </c>
       <c r="AX38" s="7">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="AY38" s="5">
         <v>0</v>
       </c>
       <c r="AZ38">
         <f t="shared" si="21"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:52">
@@ -5269,14 +5274,14 @@
         <v>2.5</v>
       </c>
       <c r="AX39" s="7">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="AY39" s="5">
         <v>0</v>
       </c>
       <c r="AZ39">
         <f t="shared" si="21"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:52">
@@ -5328,7 +5333,7 @@
       </c>
       <c r="AZ40" s="12">
         <f t="shared" ref="AZ40" si="22">SUM(AZ36:AZ39)</f>
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:52">
@@ -6139,7 +6144,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="M21" sqref="A1:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6204,7 +6209,9 @@
       <c r="C3" s="18">
         <v>0.27</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="18">
+        <v>0.94</v>
+      </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -6218,6 +6225,9 @@
       <c r="L3" s="6">
         <v>82.5</v>
       </c>
+      <c r="M3">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="7" t="s">
@@ -6229,7 +6239,9 @@
       <c r="C4" s="18">
         <v>0.57299999999999995</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="18">
+        <v>0.76600000000000001</v>
+      </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
@@ -6243,6 +6255,9 @@
       <c r="L4">
         <v>77.5</v>
       </c>
+      <c r="M4">
+        <v>119.5</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
@@ -6254,7 +6269,9 @@
       <c r="C5" s="18">
         <v>0.95</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -6267,6 +6284,9 @@
       <c r="L5">
         <v>4.5</v>
       </c>
+      <c r="M5">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
@@ -6278,7 +6298,9 @@
       <c r="C6" s="18">
         <v>0.95</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -6291,6 +6313,9 @@
       <c r="L6">
         <v>4.5</v>
       </c>
+      <c r="M6">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
@@ -6302,7 +6327,9 @@
       <c r="C7" s="18">
         <v>0.95</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -6315,6 +6342,9 @@
       <c r="L7">
         <v>18.5</v>
       </c>
+      <c r="M7">
+        <v>22.5</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
@@ -6326,7 +6356,9 @@
       <c r="C8" s="18">
         <v>0.95</v>
       </c>
-      <c r="D8" s="18"/>
+      <c r="D8" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -6339,6 +6371,9 @@
       <c r="L8">
         <v>6</v>
       </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
@@ -6350,7 +6385,9 @@
       <c r="C9" s="18">
         <v>0.5</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="18">
+        <v>0.75</v>
+      </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -6363,6 +6400,9 @@
       <c r="L9">
         <v>27</v>
       </c>
+      <c r="M9">
+        <v>39.5</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
@@ -6374,7 +6414,9 @@
       <c r="C10" s="18">
         <v>0.95</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -6387,6 +6429,9 @@
       <c r="L10">
         <v>2</v>
       </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
@@ -6398,7 +6443,9 @@
       <c r="C11" s="18">
         <v>0.7</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="18">
+        <v>0.95</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -6411,6 +6458,9 @@
       <c r="L11">
         <v>15</v>
       </c>
+      <c r="M11">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
@@ -6422,7 +6472,9 @@
       <c r="C12" s="18">
         <v>0</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="18">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
@@ -6435,6 +6487,9 @@
       <c r="L12">
         <v>0</v>
       </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
@@ -6446,7 +6501,9 @@
       <c r="C13" s="18">
         <v>0</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="18">
+        <v>0</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -6459,6 +6516,9 @@
       <c r="L13">
         <v>0</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
@@ -6470,7 +6530,9 @@
       <c r="C14" s="18">
         <v>0</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="18">
+        <v>0.7</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -6483,6 +6545,9 @@
       <c r="L14">
         <v>0</v>
       </c>
+      <c r="M14">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
@@ -6494,7 +6559,9 @@
       <c r="C15" s="18">
         <v>0</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="18">
+        <v>1</v>
+      </c>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -6507,6 +6574,9 @@
       <c r="L15">
         <v>0</v>
       </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="7" t="s">
@@ -6518,7 +6588,9 @@
       <c r="C16" s="18">
         <v>0.505</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="18">
+        <v>1</v>
+      </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -6532,8 +6604,11 @@
       <c r="L16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -6543,7 +6618,9 @@
       <c r="C17" s="18">
         <v>1</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -6556,8 +6633,11 @@
       <c r="L17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -6567,7 +6647,9 @@
       <c r="C18" s="18">
         <v>0</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="18">
+        <v>1</v>
+      </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -6580,8 +6662,11 @@
       <c r="L18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="7" t="s">
         <v>90</v>
       </c>
@@ -6591,7 +6676,9 @@
       <c r="C19" s="18">
         <v>0</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="18">
+        <v>1</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -6604,8 +6691,11 @@
       <c r="L19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -6615,7 +6705,9 @@
       <c r="C20" s="18">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
+      <c r="D20" s="18">
+        <v>1</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -6628,8 +6720,11 @@
       <c r="L20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -6639,7 +6734,9 @@
       <c r="C21" s="18">
         <v>1</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="18">
+        <v>1</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -6652,6 +6749,9 @@
       <c r="L21">
         <v>2</v>
       </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Time Chart & Started L4
</commit_message>
<xml_diff>
--- a/Reports/Time_Chart.xlsx
+++ b/Reports/Time_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11415" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Progress" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="125">
   <si>
     <t>L1</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Week 21</t>
   </si>
   <si>
-    <t>Week 22</t>
-  </si>
-  <si>
     <t>Percentage done</t>
   </si>
   <si>
@@ -337,6 +334,63 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>Post Mortem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Update Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Update UML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Team Evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Project Summary</t>
+  </si>
+  <si>
+    <t>Oral Presentation</t>
+  </si>
+  <si>
+    <t>L4-00</t>
+  </si>
+  <si>
+    <t>L4-01</t>
+  </si>
+  <si>
+    <t>L4-01a</t>
+  </si>
+  <si>
+    <t>L4-01b</t>
+  </si>
+  <si>
+    <t>L4-01c</t>
+  </si>
+  <si>
+    <t>L4-01d</t>
+  </si>
+  <si>
+    <t>L4-02</t>
+  </si>
+  <si>
+    <t>L4-03</t>
+  </si>
+  <si>
+    <t>L4-04</t>
+  </si>
+  <si>
+    <t>L4-05</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>"R8"</t>
   </si>
 </sst>
 </file>
@@ -400,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -431,6 +485,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I38" sqref="A19:I38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1769,6 +1824,329 @@
       </c>
       <c r="I38" s="7"/>
     </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="1">
+        <v>41043</v>
+      </c>
+      <c r="E41" s="1">
+        <v>41057</v>
+      </c>
+      <c r="F41">
+        <f>F42+F50+F47+F48+F49</f>
+        <v>4</v>
+      </c>
+      <c r="G41" s="14">
+        <f>(G42+G50+G47+G48+G49)/5</f>
+        <v>1.2</v>
+      </c>
+      <c r="H41">
+        <f>H42+H50+H47+H48+H49</f>
+        <v>145</v>
+      </c>
+      <c r="I41" s="14">
+        <f>I42+I50+I47+I48+I49</f>
+        <v>171.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="15">
+        <v>41043</v>
+      </c>
+      <c r="E42" s="15">
+        <v>41054</v>
+      </c>
+      <c r="F42" s="7">
+        <f>F43+F44+F45+F46</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="7">
+        <f>SUM(G43:G46)/4</f>
+        <v>1</v>
+      </c>
+      <c r="H42" s="7">
+        <f>SUM(H43:H46)</f>
+        <v>105</v>
+      </c>
+      <c r="I42" s="16">
+        <f>(SUM(I43:I46))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="1">
+        <v>41043</v>
+      </c>
+      <c r="E43" s="1">
+        <v>41050</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="I43" s="14">
+        <f>(F43/G43*100) - F43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="1">
+        <v>41043</v>
+      </c>
+      <c r="E44" s="1">
+        <v>41050</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>30</v>
+      </c>
+      <c r="I44" s="14">
+        <f t="shared" ref="I44:I49" si="3">(F44/G44*100) - F44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="1">
+        <v>41050</v>
+      </c>
+      <c r="E45" s="1">
+        <v>41054</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>25</v>
+      </c>
+      <c r="I45" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="1">
+        <v>41050</v>
+      </c>
+      <c r="E46" s="1">
+        <v>41054</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>30</v>
+      </c>
+      <c r="I46" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="15">
+        <v>41043</v>
+      </c>
+      <c r="E47" s="15">
+        <v>41054</v>
+      </c>
+      <c r="F47" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G47" s="7">
+        <v>2</v>
+      </c>
+      <c r="H47" s="7">
+        <v>10</v>
+      </c>
+      <c r="I47" s="16">
+        <f>(F47/G47*100) - F47</f>
+        <v>171.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="15">
+        <v>41043</v>
+      </c>
+      <c r="E48" s="15">
+        <v>41057</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7">
+        <v>5</v>
+      </c>
+      <c r="I48" s="7">
+        <f>(F48/G48*100) - F48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="15">
+        <v>41043</v>
+      </c>
+      <c r="E49" s="15">
+        <v>41057</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="7">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7">
+        <v>5</v>
+      </c>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="15">
+        <v>41050</v>
+      </c>
+      <c r="E50" s="15">
+        <v>41057</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="7">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7">
+        <v>20</v>
+      </c>
+      <c r="I50" s="16">
+        <f>(F50/G50*100) - F50</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1777,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ64"/>
+  <dimension ref="A1:BH64"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AZ40" sqref="AT1:AZ40"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BC15" sqref="BC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1818,7 +2196,7 @@
     <col min="43" max="43" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1847,16 +2225,22 @@
         <v>97</v>
       </c>
       <c r="AL1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AT1" t="s">
         <v>98</v>
       </c>
       <c r="AU1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52">
+        <v>104</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -1875,8 +2259,11 @@
       <c r="AV2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:52">
+      <c r="BD2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -1967,8 +2354,23 @@
       <c r="AY3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:52">
+      <c r="BC3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2131,29 +2533,56 @@
         <f>SUM(AU4:AY4)</f>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:52">
+      <c r="BB4" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC4" s="7">
+        <f t="shared" ref="BC4:BG4" si="5">SUM(BC12,BC20,BC28,BC36)</f>
+        <v>1</v>
+      </c>
+      <c r="BD4" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BE4" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BF4" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BG4" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BH4">
+        <f>SUM(BC4:BG4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:E8" si="5">(B13+B21+B29+B37+B45+B53)</f>
+        <f t="shared" ref="B5:E8" si="6">(B13+B21+B29+B37+B45+B53)</f>
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F7" si="6">(F13+F21+F29+F37+F45)</f>
+        <f t="shared" ref="F5:F7" si="7">(F13+F21+F29+F37+F45)</f>
         <v>0</v>
       </c>
       <c r="G5" s="4">
@@ -2164,23 +2593,23 @@
         <v>17</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:O7" si="7">(K13+K21+K29+K37+K45)</f>
+        <f t="shared" ref="K5:O7" si="8">(K13+K21+K29+K37+K45)</f>
         <v>0</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.6</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P5">
@@ -2191,23 +2620,23 @@
         <v>17</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" ref="T5:X5" si="8">(T13+T21+T29+T37+T45+T53+T61)</f>
+        <f t="shared" ref="T5:X5" si="9">(T13+T21+T29+T37+T45+T53+T61)</f>
         <v>3.5</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.5</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Y5">
@@ -2249,23 +2678,23 @@
         <v>3</v>
       </c>
       <c r="AM5">
-        <f t="shared" ref="AM5:AQ5" si="9">SUM(AM13,AM21,AM29,AM37)</f>
+        <f t="shared" ref="AM5:AQ5" si="10">SUM(AM13,AM21,AM29,AM37)</f>
         <v>1</v>
       </c>
       <c r="AN5" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AO5" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AP5" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="AT5" t="s">
@@ -2295,29 +2724,56 @@
         <f>SUM(AU5:AY5)</f>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:52">
+      <c r="BB5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC5" s="7">
+        <f t="shared" ref="BC5:BG5" si="11">SUM(BC13,BC21,BC29,BC37)</f>
+        <v>1</v>
+      </c>
+      <c r="BD5" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BE5" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BF5" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BG5" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BH5">
+        <f>SUM(BC5:BG5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G6" s="4">
@@ -2328,23 +2784,23 @@
         <v>18</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.1</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P6">
@@ -2355,23 +2811,23 @@
         <v>18</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" ref="T6:X6" si="10">(T14+T22+T30+T38+T46+T54+T62)</f>
+        <f t="shared" ref="T6:X6" si="12">(T14+T22+T30+T38+T46+T54+T62)</f>
         <v>3.5</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="V6" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="W6" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="Y6">
@@ -2413,23 +2869,23 @@
         <v>4</v>
       </c>
       <c r="AM6" s="7">
-        <f t="shared" ref="AM6:AQ6" si="11">SUM(AM22,AM30,AM38,AM14)</f>
+        <f t="shared" ref="AM6:AQ6" si="13">SUM(AM22,AM30,AM38,AM14)</f>
         <v>2</v>
       </c>
       <c r="AN6" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="AO6" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="AP6" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>20.5</v>
       </c>
       <c r="AT6" t="s">
@@ -2459,29 +2915,56 @@
         <f>SUM(AU6:AY6)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:52">
+      <c r="BB6" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC6" s="7">
+        <f>SUM(BC22,BC30,BC38,BC14)</f>
+        <v>1</v>
+      </c>
+      <c r="BD6" s="5">
+        <f>SUM(BD22,BD30,BD38,BD14)</f>
+        <v>0</v>
+      </c>
+      <c r="BE6" s="5">
+        <f>SUM(BE22,BE30,BE38,BE14)</f>
+        <v>0</v>
+      </c>
+      <c r="BF6" s="5">
+        <f>SUM(BF22,BF30,BF38,BF14)</f>
+        <v>0</v>
+      </c>
+      <c r="BG6" s="5">
+        <f>SUM(BG22,BG30,BG38,BG14)</f>
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <f>SUM(BC6:BG6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G7" s="4">
@@ -2492,23 +2975,23 @@
         <v>15</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.1</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P7">
@@ -2519,23 +3002,23 @@
         <v>15</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" ref="T7:X7" si="12">(T15+T23+T31+T39+T47+T55+T63)</f>
+        <f t="shared" ref="T7:X7" si="14">(T15+T23+T31+T39+T47+T55+T63)</f>
         <v>3.5</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="V7" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="W7" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.5</v>
       </c>
       <c r="Y7">
@@ -2577,23 +3060,23 @@
         <v>3</v>
       </c>
       <c r="AM7">
-        <f t="shared" ref="AM7:AQ7" si="13">SUM(AM15,AM23,AM31,AM39)</f>
+        <f t="shared" ref="AM7:AQ7" si="15">SUM(AM15,AM23,AM31,AM39)</f>
         <v>0</v>
       </c>
       <c r="AN7" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AO7" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AP7" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>13</v>
       </c>
       <c r="AT7" t="s">
@@ -2623,25 +3106,52 @@
         <f>SUM(AU7:AY7)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:52">
+      <c r="BB7" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC7" s="7">
+        <f>SUM(BC15,BC23,BC31,BC39)</f>
+        <v>1</v>
+      </c>
+      <c r="BD7" s="5">
+        <f>SUM(BD15,BD23,BD31,BD39)</f>
+        <v>0</v>
+      </c>
+      <c r="BE7" s="5">
+        <f>SUM(BE15,BE23,BE31,BE39)</f>
+        <v>0</v>
+      </c>
+      <c r="BF7" s="5">
+        <f>SUM(BF15,BF23,BF31,BF39)</f>
+        <v>0</v>
+      </c>
+      <c r="BG7" s="5">
+        <f>SUM(BG15,BG23,BG31,BG39)</f>
+        <v>0</v>
+      </c>
+      <c r="BH7">
+        <f>SUM(BC7:BG7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -2684,17 +3194,21 @@
         <v>61</v>
       </c>
       <c r="AZ8" s="12">
-        <f t="shared" ref="AZ8" si="14">SUM(AZ4:AZ7)</f>
+        <f t="shared" ref="AZ8" si="16">SUM(AZ4:AZ7)</f>
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:52">
+      <c r="BH8" s="12">
+        <f t="shared" ref="BH8" si="17">SUM(BH4:BH7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60">
       <c r="G9" s="11">
         <f>SUM(G4:G8)</f>
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:60">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -2714,8 +3228,11 @@
       <c r="AV10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:52">
+      <c r="BD10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>36</v>
@@ -2808,8 +3325,23 @@
       <c r="AY11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:52">
+      <c r="BC11" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE11" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2927,11 +3459,25 @@
         <v>0</v>
       </c>
       <c r="AZ12">
-        <f t="shared" ref="AZ12:AZ15" si="15">SUM(AU12:AY12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:52">
+        <f t="shared" ref="AZ12:AZ15" si="18">SUM(AU12:AY12)</f>
+        <v>0</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC12" s="7">
+        <v>1</v>
+      </c>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="5"/>
+      <c r="BF12" s="5"/>
+      <c r="BG12" s="5"/>
+      <c r="BH12">
+        <f t="shared" ref="BH12:BH15" si="19">SUM(BC12:BG12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -3049,11 +3595,25 @@
         <v>0</v>
       </c>
       <c r="AZ13">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:52">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC13" s="7">
+        <v>1</v>
+      </c>
+      <c r="BD13" s="5"/>
+      <c r="BE13" s="5"/>
+      <c r="BF13" s="5"/>
+      <c r="BG13" s="5"/>
+      <c r="BH13">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -3174,11 +3734,25 @@
         <v>1</v>
       </c>
       <c r="AZ14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:52">
+      <c r="BB14" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC14" s="7">
+        <v>1</v>
+      </c>
+      <c r="BD14" s="5"/>
+      <c r="BE14" s="5"/>
+      <c r="BF14" s="5"/>
+      <c r="BG14" s="5"/>
+      <c r="BH14">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -3296,11 +3870,25 @@
         <v>0</v>
       </c>
       <c r="AZ15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:52">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC15" s="7">
+        <v>1</v>
+      </c>
+      <c r="BD15" s="5"/>
+      <c r="BE15" s="5"/>
+      <c r="BF15" s="5"/>
+      <c r="BG15" s="5"/>
+      <c r="BH15">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:60">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -3353,11 +3941,15 @@
         <v>5</v>
       </c>
       <c r="AZ16" s="12">
-        <f t="shared" ref="AZ16" si="16">SUM(AZ12:AZ15)</f>
+        <f t="shared" ref="AZ16" si="20">SUM(AZ12:AZ15)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:52">
+      <c r="BH16" s="12">
+        <f t="shared" ref="BH16" si="21">SUM(BH12:BH15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:60">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3369,7 +3961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:52">
+    <row r="18" spans="1:60">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -3394,8 +3986,11 @@
       <c r="AV18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:52">
+      <c r="BD18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:60">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -3488,8 +4083,23 @@
       <c r="AY19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:52">
+      <c r="BC19" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:60">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
@@ -3602,11 +4212,23 @@
         <v>0</v>
       </c>
       <c r="AZ20">
-        <f t="shared" ref="AZ20:AZ23" si="17">SUM(AU20:AY20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:52">
+        <f t="shared" ref="AZ20:AZ23" si="22">SUM(AU20:AY20)</f>
+        <v>0</v>
+      </c>
+      <c r="BB20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC20" s="5"/>
+      <c r="BD20" s="5"/>
+      <c r="BE20" s="5"/>
+      <c r="BF20" s="5"/>
+      <c r="BG20" s="5"/>
+      <c r="BH20">
+        <f t="shared" ref="BH20:BH23" si="23">SUM(BC20:BG20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:60">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -3719,11 +4341,23 @@
         <v>0</v>
       </c>
       <c r="AZ21">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:52">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC21" s="5"/>
+      <c r="BD21" s="5"/>
+      <c r="BE21" s="5"/>
+      <c r="BF21" s="5"/>
+      <c r="BG21" s="5"/>
+      <c r="BH21">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:60">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
@@ -3836,11 +4470,23 @@
         <v>1</v>
       </c>
       <c r="AZ22">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:52">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="BB22" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC22" s="5"/>
+      <c r="BD22" s="5"/>
+      <c r="BE22" s="5"/>
+      <c r="BF22" s="5"/>
+      <c r="BG22" s="5"/>
+      <c r="BH22">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:60">
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
@@ -3953,11 +4599,23 @@
         <v>0</v>
       </c>
       <c r="AZ23">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:52">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC23" s="5"/>
+      <c r="BD23" s="5"/>
+      <c r="BE23" s="5"/>
+      <c r="BF23" s="5"/>
+      <c r="BG23" s="5"/>
+      <c r="BH23">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:60">
       <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
@@ -4012,11 +4670,15 @@
         <v>0</v>
       </c>
       <c r="AZ24" s="12">
-        <f t="shared" ref="AZ24" si="18">SUM(AZ20:AZ23)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:52">
+        <f t="shared" ref="AZ24" si="24">SUM(AZ20:AZ23)</f>
+        <v>1</v>
+      </c>
+      <c r="BH24" s="12">
+        <f t="shared" ref="BH24" si="25">SUM(BH20:BH23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:60">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -4028,7 +4690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:52">
+    <row r="26" spans="1:60">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -4053,8 +4715,11 @@
       <c r="AV26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:52">
+      <c r="BD26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:60">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>36</v>
@@ -4147,8 +4812,23 @@
       <c r="AY27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:52">
+      <c r="BC27" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD27" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE27" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF27" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:60">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -4264,11 +4944,23 @@
         <v>0</v>
       </c>
       <c r="AZ28">
-        <f t="shared" ref="AZ28:AZ31" si="19">SUM(AU28:AY28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:52">
+        <f t="shared" ref="AZ28:AZ31" si="26">SUM(AU28:AY28)</f>
+        <v>0</v>
+      </c>
+      <c r="BB28" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC28" s="5"/>
+      <c r="BD28" s="5"/>
+      <c r="BE28" s="5"/>
+      <c r="BF28" s="5"/>
+      <c r="BG28" s="5"/>
+      <c r="BH28">
+        <f t="shared" ref="BH28:BH31" si="27">SUM(BC28:BG28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:60">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -4377,11 +5069,23 @@
         <v>0</v>
       </c>
       <c r="AZ29">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:52">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="BB29" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC29" s="5"/>
+      <c r="BD29" s="5"/>
+      <c r="BE29" s="5"/>
+      <c r="BF29" s="5"/>
+      <c r="BG29" s="5"/>
+      <c r="BH29">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:60">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -4490,11 +5194,23 @@
         <v>0</v>
       </c>
       <c r="AZ30">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:52">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC30" s="5"/>
+      <c r="BD30" s="5"/>
+      <c r="BE30" s="5"/>
+      <c r="BF30" s="5"/>
+      <c r="BG30" s="5"/>
+      <c r="BH30">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:60">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
@@ -4607,11 +5323,23 @@
         <v>0</v>
       </c>
       <c r="AZ31">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:52">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="BB31" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC31" s="5"/>
+      <c r="BD31" s="5"/>
+      <c r="BE31" s="5"/>
+      <c r="BF31" s="5"/>
+      <c r="BG31" s="5"/>
+      <c r="BH31">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60">
       <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
@@ -4666,11 +5394,15 @@
         <v>0</v>
       </c>
       <c r="AZ32" s="12">
-        <f t="shared" ref="AZ32" si="20">SUM(AZ28:AZ31)</f>
+        <f t="shared" ref="AZ32" si="28">SUM(AZ28:AZ31)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:52">
+      <c r="BH32" s="12">
+        <f t="shared" ref="BH32" si="29">SUM(BH28:BH31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:60">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -4682,7 +5414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:52">
+    <row r="34" spans="1:60">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -4702,19 +5434,25 @@
         <v>5</v>
       </c>
       <c r="AK34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AM34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AT34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AV34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:52">
+        <v>103</v>
+      </c>
+      <c r="BB34" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:60">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
@@ -4807,8 +5545,23 @@
       <c r="AY35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:52">
+      <c r="BC35" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD35" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE35" t="s">
+        <v>38</v>
+      </c>
+      <c r="BF35" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:60">
       <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
@@ -4922,11 +5675,23 @@
         <v>0</v>
       </c>
       <c r="AZ36">
-        <f t="shared" ref="AZ36:AZ39" si="21">SUM(AU36:AY36)</f>
+        <f t="shared" ref="AZ36:AZ39" si="30">SUM(AU36:AY36)</f>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:52">
+      <c r="BB36" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC36" s="5"/>
+      <c r="BD36" s="5"/>
+      <c r="BE36" s="5"/>
+      <c r="BF36" s="5"/>
+      <c r="BG36" s="5"/>
+      <c r="BH36">
+        <f t="shared" ref="BH36:BH39" si="31">SUM(BC36:BG36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:60">
       <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
@@ -5044,11 +5809,23 @@
         <v>0</v>
       </c>
       <c r="AZ37">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:52">
+      <c r="BB37" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC37" s="5"/>
+      <c r="BD37" s="5"/>
+      <c r="BE37" s="5"/>
+      <c r="BF37" s="5"/>
+      <c r="BG37" s="5"/>
+      <c r="BH37">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:60">
       <c r="A38" s="5" t="s">
         <v>18</v>
       </c>
@@ -5162,11 +5939,23 @@
         <v>0</v>
       </c>
       <c r="AZ38">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:52">
+      <c r="BB38" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC38" s="5"/>
+      <c r="BD38" s="5"/>
+      <c r="BE38" s="5"/>
+      <c r="BF38" s="5"/>
+      <c r="BG38" s="5"/>
+      <c r="BH38">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:60">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -5280,11 +6069,23 @@
         <v>0</v>
       </c>
       <c r="AZ39">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:52">
+      <c r="BB39" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC39" s="5"/>
+      <c r="BD39" s="5"/>
+      <c r="BE39" s="5"/>
+      <c r="BF39" s="5"/>
+      <c r="BG39" s="5"/>
+      <c r="BH39">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:60">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -5332,11 +6133,15 @@
         <v>56</v>
       </c>
       <c r="AZ40" s="12">
-        <f t="shared" ref="AZ40" si="22">SUM(AZ36:AZ39)</f>
+        <f t="shared" ref="AZ40" si="32">SUM(AZ36:AZ39)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:52">
+      <c r="BH40" s="12">
+        <f t="shared" ref="BH40" si="33">SUM(BH36:BH39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:60">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -5348,7 +6153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:52">
+    <row r="42" spans="1:60">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -5368,7 +6173,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:52">
+    <row r="43" spans="1:60">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>36</v>
@@ -5432,7 +6237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:52">
+    <row r="44" spans="1:60">
       <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
@@ -5503,7 +6308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:52">
+    <row r="45" spans="1:60">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -5574,7 +6379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:52">
+    <row r="46" spans="1:60">
       <c r="A46" s="5" t="s">
         <v>18</v>
       </c>
@@ -5645,7 +6450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:52">
+    <row r="47" spans="1:60">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -5716,7 +6521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:52">
+    <row r="48" spans="1:60">
       <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
@@ -6141,27 +6946,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="A1:M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
         <v>88</v>
       </c>
@@ -6171,35 +6977,17 @@
       <c r="D2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>100</v>
-      </c>
       <c r="G2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K2" t="s">
         <v>88</v>
       </c>
-      <c r="L2" t="s">
+      <c r="H2" t="s">
         <v>97</v>
       </c>
-      <c r="M2" t="s">
+      <c r="I2" t="s">
         <v>98</v>
       </c>
-      <c r="N2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" t="s">
-        <v>100</v>
-      </c>
-      <c r="P2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6213,23 +7001,21 @@
         <v>0.94</v>
       </c>
       <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="J3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="K3">
-        <f>K4+K15+K16+K19+K20+K21</f>
+      <c r="G3">
+        <f>G4+G15+G16+G19+G20+G21</f>
         <v>21</v>
       </c>
-      <c r="L3" s="6">
+      <c r="H3" s="6">
         <v>82.5</v>
       </c>
-      <c r="M3">
+      <c r="I3">
         <v>131.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
@@ -6243,23 +7029,21 @@
         <v>0.76600000000000001</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="J4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="7">
-        <f>SUM(K5:K14)</f>
+      <c r="G4" s="7">
+        <f>SUM(G5:G14)</f>
         <v>21</v>
       </c>
-      <c r="L4">
+      <c r="H4">
         <v>77.5</v>
       </c>
-      <c r="M4">
+      <c r="I4">
         <v>119.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -6273,22 +7057,20 @@
         <v>0.95</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="J5" t="s">
+      <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="K5">
+      <c r="G5">
         <v>1.5</v>
       </c>
-      <c r="L5">
+      <c r="H5">
         <v>4.5</v>
       </c>
-      <c r="M5">
+      <c r="I5">
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -6302,22 +7084,20 @@
         <v>0.95</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="J6" t="s">
+      <c r="F6" t="s">
         <v>95</v>
       </c>
-      <c r="K6">
+      <c r="G6">
         <v>0.5</v>
       </c>
-      <c r="L6">
+      <c r="H6">
         <v>4.5</v>
       </c>
-      <c r="M6">
+      <c r="I6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -6331,22 +7111,20 @@
         <v>0.95</v>
       </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="J7" t="s">
+      <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="K7">
+      <c r="G7">
         <v>12.5</v>
       </c>
-      <c r="L7">
+      <c r="H7">
         <v>18.5</v>
       </c>
-      <c r="M7">
+      <c r="I7">
         <v>22.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -6360,22 +7138,20 @@
         <v>0.95</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="J8" t="s">
+      <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="K8">
+      <c r="G8">
         <v>4</v>
       </c>
-      <c r="L8">
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="I8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -6389,22 +7165,20 @@
         <v>0.75</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="J9" t="s">
+      <c r="F9" t="s">
         <v>55</v>
       </c>
-      <c r="K9">
+      <c r="G9">
         <v>2.5</v>
       </c>
-      <c r="L9">
+      <c r="H9">
         <v>27</v>
       </c>
-      <c r="M9">
+      <c r="I9">
         <v>39.5</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -6418,22 +7192,20 @@
         <v>0.95</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="J10" t="s">
+      <c r="F10" t="s">
         <v>56</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="M10">
+      <c r="I10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -6447,22 +7219,20 @@
         <v>0.95</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="J11" t="s">
+      <c r="F11" t="s">
         <v>63</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>15</v>
       </c>
-      <c r="M11">
+      <c r="I11">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -6476,22 +7246,20 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="J12" t="s">
+      <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -6505,22 +7273,20 @@
         <v>0</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="J13" t="s">
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -6534,22 +7300,20 @@
         <v>0.7</v>
       </c>
       <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="J14" t="s">
+      <c r="F14" t="s">
         <v>94</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
@@ -6563,22 +7327,20 @@
         <v>1</v>
       </c>
       <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="J15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="7">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -6592,23 +7354,21 @@
         <v>1</v>
       </c>
       <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="J16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="7">
-        <f>SUM(K17:K18)</f>
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="G16" s="7">
+        <f>SUM(G17:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="M16">
+      <c r="I16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -6622,22 +7382,20 @@
         <v>1</v>
       </c>
       <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="J17" t="s">
+      <c r="F17" t="s">
         <v>70</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>3</v>
       </c>
-      <c r="M17">
+      <c r="I17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -6651,22 +7409,20 @@
         <v>1</v>
       </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="J18" t="s">
+      <c r="F18" t="s">
         <v>71</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:9">
       <c r="A19" s="7" t="s">
         <v>90</v>
       </c>
@@ -6680,22 +7436,20 @@
         <v>1</v>
       </c>
       <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="K19" s="7">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -6709,22 +7463,20 @@
         <v>1</v>
       </c>
       <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="J20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20">
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>2</v>
       </c>
-      <c r="M20">
+      <c r="I20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -6738,20 +7490,233 @@
         <v>1</v>
       </c>
       <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="J21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="7">
-        <v>0</v>
-      </c>
-      <c r="L21">
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>2</v>
       </c>
-      <c r="M21">
+      <c r="I21">
         <v>2</v>
       </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="5"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="5"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="5"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>